<commit_message>
v6.alpha Add from txt url
</commit_message>
<xml_diff>
--- a/Geocoding.xlsx
+++ b/Geocoding.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B119"/>
+  <dimension ref="A1:B358"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -423,954 +423,2866 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="n">
-        <v>37.794181</v>
+        <v>60.047236</v>
       </c>
       <c r="B1" t="n">
-        <v>55.703682</v>
+        <v>30.451109</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>37.552058</v>
+        <v>60.047236</v>
       </c>
       <c r="B2" t="n">
-        <v>55.942766</v>
+        <v>30.451109</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>37.632592</v>
+        <v>60.047236</v>
       </c>
       <c r="B3" t="n">
-        <v>55.80187</v>
+        <v>30.451109</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>37.803281</v>
+        <v>60.018839</v>
       </c>
       <c r="B4" t="n">
-        <v>55.793541</v>
+        <v>30.432685</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>37.600774</v>
+        <v>59.930629</v>
       </c>
       <c r="B5" t="n">
-        <v>55.888614</v>
+        <v>30.238505</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>37.592752</v>
+        <v>60.024131</v>
       </c>
       <c r="B6" t="n">
-        <v>55.751817</v>
+        <v>30.333843</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>37.608481</v>
+        <v>60.000267</v>
       </c>
       <c r="B7" t="n">
-        <v>55.763609</v>
+        <v>30.324366</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>38.411755</v>
+        <v>60.051284</v>
       </c>
       <c r="B8" t="n">
-        <v>55.836838</v>
+        <v>30.438578</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>37.750613</v>
+        <v>59.838186</v>
       </c>
       <c r="B9" t="n">
-        <v>55.572279</v>
+        <v>30.231346</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>37.639401</v>
+        <v>59.909617</v>
       </c>
       <c r="B10" t="n">
-        <v>55.778396</v>
+        <v>30.278498</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>37.673169</v>
+        <v>59.839353</v>
       </c>
       <c r="B11" t="n">
-        <v>55.873521</v>
+        <v>30.239664</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>37.732467</v>
+        <v>59.856352</v>
       </c>
       <c r="B12" t="n">
-        <v>55.766207</v>
+        <v>30.197201</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>37.35336</v>
+        <v>59.91069</v>
       </c>
       <c r="B13" t="n">
-        <v>55.809879</v>
+        <v>30.31161</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>37.852868</v>
+        <v>60.05909</v>
       </c>
       <c r="B14" t="n">
-        <v>56.043005</v>
+        <v>30.335029</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>37.568479</v>
+        <v>60.077135</v>
       </c>
       <c r="B15" t="n">
-        <v>55.859443</v>
+        <v>30.252833</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>37.440407</v>
+        <v>59.859976</v>
       </c>
       <c r="B16" t="n">
-        <v>55.683843</v>
+        <v>30.178417</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>37.898071</v>
+        <v>59.83843</v>
       </c>
       <c r="B17" t="n">
-        <v>55.655579</v>
+        <v>30.204459</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>37.650738</v>
+        <v>59.930007</v>
       </c>
       <c r="B18" t="n">
-        <v>55.665599</v>
+        <v>30.315293</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>37.354644</v>
+        <v>59.901247</v>
       </c>
       <c r="B19" t="n">
-        <v>55.836777</v>
+        <v>30.487698</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>37.776646</v>
+        <v>59.942421</v>
       </c>
       <c r="B20" t="n">
-        <v>55.765154</v>
+        <v>30.283232</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>37.406289</v>
+        <v>59.937873</v>
       </c>
       <c r="B21" t="n">
-        <v>55.803737</v>
+        <v>30.305852</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>37.342894</v>
+        <v>59.93245</v>
       </c>
       <c r="B22" t="n">
-        <v>55.739422</v>
+        <v>30.349267</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>37.409163</v>
+        <v>59.904947</v>
       </c>
       <c r="B23" t="n">
-        <v>55.827788</v>
+        <v>30.273504</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>37.455247</v>
+        <v>59.9496</v>
       </c>
       <c r="B24" t="n">
-        <v>55.796835</v>
+        <v>30.305034</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>37.616692</v>
+        <v>59.922706</v>
       </c>
       <c r="B25" t="n">
-        <v>55.849676</v>
+        <v>30.458772</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>37.281117</v>
+        <v>60.044859</v>
       </c>
       <c r="B26" t="n">
-        <v>55.942499</v>
+        <v>30.351055</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>38.034651</v>
+        <v>60.081785</v>
       </c>
       <c r="B27" t="n">
-        <v>55.748052</v>
+        <v>30.248944</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>37.485601</v>
+        <v>59.909265</v>
       </c>
       <c r="B28" t="n">
-        <v>55.499183</v>
+        <v>30.312598</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>37.677014</v>
+        <v>59.901247</v>
       </c>
       <c r="B29" t="n">
-        <v>55.723577</v>
+        <v>30.487698</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>37.747496</v>
+        <v>59.930007</v>
       </c>
       <c r="B30" t="n">
-        <v>55.670854</v>
+        <v>30.315293</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>37.892951</v>
+        <v>59.920492</v>
       </c>
       <c r="B31" t="n">
-        <v>55.3235</v>
+        <v>30.359077</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>37.539949</v>
+        <v>59.90418</v>
       </c>
       <c r="B32" t="n">
-        <v>55.790529</v>
+        <v>30.457541</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>37.851116</v>
+        <v>60.072296</v>
       </c>
       <c r="B33" t="n">
-        <v>55.325206</v>
+        <v>30.362212</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>38.069694</v>
+        <v>59.977012</v>
       </c>
       <c r="B34" t="n">
-        <v>55.632916</v>
+        <v>30.331741</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>37.709901</v>
+        <v>59.979056</v>
       </c>
       <c r="B35" t="n">
-        <v>55.555958</v>
+        <v>30.337149</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>37.292436</v>
+        <v>60.051181</v>
       </c>
       <c r="B36" t="n">
-        <v>55.610478</v>
+        <v>30.333879</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>37.659452</v>
+        <v>60.028928</v>
       </c>
       <c r="B37" t="n">
-        <v>55.734004</v>
+        <v>30.330511</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>38.578815</v>
+        <v>60.00029</v>
       </c>
       <c r="B38" t="n">
-        <v>55.34128</v>
+        <v>30.316254</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>37.837264</v>
+        <v>59.943701</v>
       </c>
       <c r="B39" t="n">
-        <v>55.38686</v>
+        <v>30.371267</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>37.924392</v>
+        <v>59.842033</v>
       </c>
       <c r="B40" t="n">
-        <v>55.660323</v>
+        <v>30.131237</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>37.576241</v>
+        <v>59.967155</v>
       </c>
       <c r="B41" t="n">
-        <v>55.801546</v>
+        <v>30.273737</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>37.866891</v>
+        <v>59.968232</v>
       </c>
       <c r="B42" t="n">
-        <v>55.624556</v>
+        <v>30.308843</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>37.269305</v>
+        <v>59.833059</v>
       </c>
       <c r="B43" t="n">
-        <v>55.671097</v>
+        <v>30.173746</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>37.113968</v>
+        <v>59.854332</v>
       </c>
       <c r="B44" t="n">
-        <v>55.857397</v>
+        <v>30.387437</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>30.202052</v>
+        <v>59.965241</v>
       </c>
       <c r="B45" t="n">
-        <v>60.380048</v>
+        <v>30.406948</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>37.496246</v>
+        <v>60.041516</v>
       </c>
       <c r="B46" t="n">
-        <v>55.931255</v>
+        <v>30.318994</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>38.136224</v>
+        <v>60.084289</v>
       </c>
       <c r="B47" t="n">
-        <v>55.589671</v>
+        <v>30.267332</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>37.689932</v>
+        <v>59.84819</v>
       </c>
       <c r="B48" t="n">
-        <v>55.735713</v>
+        <v>30.40552</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>37.793624</v>
+        <v>59.952096</v>
       </c>
       <c r="B49" t="n">
-        <v>55.642738</v>
+        <v>30.436817</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>37.255911</v>
+        <v>60.047236</v>
       </c>
       <c r="B50" t="n">
-        <v>55.837616</v>
+        <v>30.451109</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>37.862633</v>
+        <v>60.047236</v>
       </c>
       <c r="B51" t="n">
-        <v>55.720413</v>
+        <v>30.451109</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>37.565856</v>
+        <v>60.018785</v>
       </c>
       <c r="B52" t="n">
-        <v>55.763614</v>
+        <v>30.280744</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>37.417536</v>
+        <v>59.938432</v>
       </c>
       <c r="B53" t="n">
-        <v>55.732175</v>
+        <v>30.212553</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>37.704071</v>
+        <v>59.929177</v>
       </c>
       <c r="B54" t="n">
-        <v>55.758792</v>
+        <v>30.364638</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="n">
-        <v>37.479582</v>
+        <v>59.938139</v>
       </c>
       <c r="B55" t="n">
-        <v>56.046308</v>
+        <v>30.47734</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="n">
-        <v>37.935351</v>
+        <v>60.013312</v>
       </c>
       <c r="B56" t="n">
-        <v>55.566028</v>
+        <v>30.36055</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="n">
-        <v>37.521686</v>
+        <v>59.928059</v>
       </c>
       <c r="B57" t="n">
-        <v>55.310227</v>
+        <v>30.305636</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
-        <v>37.738243</v>
+        <v>60.13621</v>
       </c>
       <c r="B58" t="n">
-        <v>55.673692</v>
+        <v>30.257846</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="n">
-        <v>37.736563</v>
+        <v>59.611928</v>
       </c>
       <c r="B59" t="n">
-        <v>55.658733</v>
+        <v>30.171554</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="n">
-        <v>37.729583</v>
+        <v>59.991358</v>
       </c>
       <c r="B60" t="n">
-        <v>55.894005</v>
+        <v>30.160981</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="n">
-        <v>37.037979</v>
+        <v>59.991358</v>
       </c>
       <c r="B61" t="n">
-        <v>55.672534</v>
+        <v>30.160981</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="n">
-        <v>37.170247</v>
+        <v>59.991358</v>
       </c>
       <c r="B62" t="n">
-        <v>55.848817</v>
+        <v>30.160981</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="n">
-        <v>37.92865</v>
+        <v>60.030542</v>
       </c>
       <c r="B63" t="n">
-        <v>55.681742</v>
+        <v>29.990705</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="n">
-        <v>37.453765</v>
+        <v>60.041332</v>
       </c>
       <c r="B64" t="n">
-        <v>55.892617</v>
+        <v>30.311799</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="n">
-        <v>37.256225</v>
+        <v>59.942885</v>
       </c>
       <c r="B65" t="n">
-        <v>55.841043</v>
+        <v>30.361116</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="n">
-        <v>38.011681</v>
+        <v>59.874697</v>
       </c>
       <c r="B66" t="n">
-        <v>55.661841</v>
+        <v>30.33591</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="n">
-        <v>37.900542</v>
+        <v>59.924406</v>
       </c>
       <c r="B67" t="n">
-        <v>55.589743</v>
+        <v>30.385784</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="n">
-        <v>37.533751</v>
+        <v>59.873586</v>
       </c>
       <c r="B68" t="n">
-        <v>55.41284</v>
+        <v>30.471142</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="n">
-        <v>37.763405</v>
+        <v>60.023362</v>
       </c>
       <c r="B69" t="n">
-        <v>55.680747</v>
+        <v>30.677018</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="n">
-        <v>37.580202</v>
+        <v>59.973028</v>
       </c>
       <c r="B70" t="n">
-        <v>55.457592</v>
+        <v>30.338461</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="n">
-        <v>37.842978</v>
+        <v>60.045565</v>
       </c>
       <c r="B71" t="n">
-        <v>55.913263</v>
+        <v>30.301208</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="n">
-        <v>37.449884</v>
+        <v>60.042173</v>
       </c>
       <c r="B72" t="n">
-        <v>55.677803</v>
+        <v>30.363865</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="n">
-        <v>37.711842</v>
+        <v>59.936377</v>
       </c>
       <c r="B73" t="n">
-        <v>55.895782</v>
+        <v>30.367701</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="n">
-        <v>37.545087</v>
+        <v>59.913663</v>
       </c>
       <c r="B74" t="n">
-        <v>55.409692</v>
+        <v>30.282639</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="n">
-        <v>37.508391</v>
+        <v>59.935791</v>
       </c>
       <c r="B75" t="n">
-        <v>55.744961</v>
+        <v>30.369273</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="n">
-        <v>37.854395</v>
+        <v>60.006498</v>
       </c>
       <c r="B76" t="n">
-        <v>55.764101</v>
+        <v>30.275642</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="n">
-        <v>37.631146</v>
+        <v>59.833059</v>
       </c>
       <c r="B77" t="n">
-        <v>55.786814</v>
+        <v>30.173746</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="n">
-        <v>37.489796</v>
+        <v>59.933911</v>
       </c>
       <c r="B78" t="n">
-        <v>55.440345</v>
+        <v>30.371195</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="n">
-        <v>37.554582</v>
+        <v>59.834926</v>
       </c>
       <c r="B79" t="n">
-        <v>55.347357</v>
+        <v>30.217206</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="n">
-        <v>37.699274</v>
+        <v>60.055753</v>
       </c>
       <c r="B80" t="n">
-        <v>55.556604</v>
+        <v>30.339332</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="n">
-        <v>36.982679</v>
+        <v>59.861828</v>
       </c>
       <c r="B81" t="n">
-        <v>55.738718</v>
+        <v>30.33829</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="n">
-        <v>37.958564</v>
+        <v>60.055672</v>
       </c>
       <c r="B82" t="n">
-        <v>55.812545</v>
+        <v>30.358502</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="n">
-        <v>37.622073</v>
+        <v>60.167975</v>
       </c>
       <c r="B83" t="n">
-        <v>55.764268</v>
+        <v>30.354954</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="n">
-        <v>37.528109</v>
+        <v>59.720608</v>
       </c>
       <c r="B84" t="n">
-        <v>55.839062</v>
+        <v>30.429244</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="n">
-        <v>37.531819</v>
+        <v>59.985638</v>
       </c>
       <c r="B85" t="n">
-        <v>55.772284</v>
+        <v>30.350399</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="n">
-        <v>37.742663</v>
+        <v>59.914556</v>
       </c>
       <c r="B86" t="n">
-        <v>55.669554</v>
+        <v>30.486467</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="n">
-        <v>37.628406</v>
+        <v>59.889634</v>
       </c>
       <c r="B87" t="n">
-        <v>55.775459</v>
+        <v>30.47664</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="n">
-        <v>37.617096</v>
+        <v>60.110298</v>
       </c>
       <c r="B88" t="n">
-        <v>55.890997</v>
+        <v>30.344776</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="n">
-        <v>37.522764</v>
+        <v>59.995417</v>
       </c>
       <c r="B89" t="n">
-        <v>55.633023</v>
+        <v>30.295063</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="n">
-        <v>37.474363</v>
+        <v>59.938955</v>
       </c>
       <c r="B90" t="n">
-        <v>55.731445</v>
+        <v>30.315644</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="n">
-        <v>37.62519</v>
+        <v>59.904184</v>
       </c>
       <c r="B91" t="n">
-        <v>55.660404</v>
+        <v>30.562824</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="n">
-        <v>37.632143</v>
+        <v>59.888952</v>
       </c>
       <c r="B92" t="n">
-        <v>55.742747</v>
+        <v>30.420468</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="n">
-        <v>37.796229</v>
+        <v>59.855331</v>
       </c>
       <c r="B93" t="n">
-        <v>55.745605</v>
+        <v>30.378678</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="n">
-        <v>37.583104</v>
+        <v>59.916582</v>
       </c>
       <c r="B94" t="n">
-        <v>55.573576</v>
+        <v>30.288227</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="n">
-        <v>37.701709</v>
+        <v>59.949104</v>
       </c>
       <c r="B95" t="n">
-        <v>55.863863</v>
+        <v>30.342997</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="n">
-        <v>37.794576</v>
+        <v>59.953637</v>
       </c>
       <c r="B96" t="n">
-        <v>55.799487</v>
+        <v>30.449322</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="n">
-        <v>37.78288</v>
+        <v>59.838055</v>
       </c>
       <c r="B97" t="n">
-        <v>55.816925</v>
+        <v>30.350444</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="n">
-        <v>37.53605</v>
+        <v>59.993784</v>
       </c>
       <c r="B98" t="n">
-        <v>55.845127</v>
+        <v>30.107594</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="n">
-        <v>37.771849</v>
+        <v>59.97106</v>
       </c>
       <c r="B99" t="n">
-        <v>55.730269</v>
+        <v>30.434787</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="n">
-        <v>37.574687</v>
+        <v>59.928672</v>
       </c>
       <c r="B100" t="n">
-        <v>55.720869</v>
+        <v>30.420225</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="n">
-        <v>37.606406</v>
+        <v>59.928672</v>
       </c>
       <c r="B101" t="n">
-        <v>55.706847</v>
+        <v>30.420225</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="n">
-        <v>37.591162</v>
+        <v>59.941817</v>
       </c>
       <c r="B102" t="n">
-        <v>55.831555</v>
+        <v>30.2602</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="n">
-        <v>37.474354</v>
+        <v>59.932135</v>
       </c>
       <c r="B103" t="n">
-        <v>55.864162</v>
+        <v>30.470567</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="n">
-        <v>37.76999</v>
+        <v>60.008477</v>
       </c>
       <c r="B104" t="n">
-        <v>55.808902</v>
+        <v>30.294973</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="n">
-        <v>37.498213</v>
+        <v>59.940772</v>
       </c>
       <c r="B105" t="n">
-        <v>55.868304</v>
+        <v>30.290113</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="n">
-        <v>37.471309</v>
+        <v>59.980745</v>
       </c>
       <c r="B106" t="n">
-        <v>55.784784</v>
+        <v>30.388506</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="n">
-        <v>37.607053</v>
+        <v>59.720608</v>
       </c>
       <c r="B107" t="n">
-        <v>55.780912</v>
+        <v>30.429244</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="n">
-        <v>38.008995</v>
+        <v>59.997923</v>
       </c>
       <c r="B108" t="n">
-        <v>55.919559</v>
+        <v>30.260738</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="n">
-        <v>37.083874</v>
+        <v>59.870696</v>
       </c>
       <c r="B109" t="n">
-        <v>55.812403</v>
+        <v>30.448522</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="n">
-        <v>38.257128</v>
+        <v>59.987326</v>
       </c>
       <c r="B110" t="n">
-        <v>55.551573</v>
+        <v>30.292781</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="n">
-        <v>37.581406</v>
+        <v>59.947545</v>
       </c>
       <c r="B111" t="n">
-        <v>55.602383</v>
+        <v>30.361359</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="n">
-        <v>37.57969</v>
+        <v>59.915413</v>
       </c>
       <c r="B112" t="n">
-        <v>55.841898</v>
+        <v>30.310343</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="n">
-        <v>37.447054</v>
+        <v>59.907212</v>
       </c>
       <c r="B113" t="n">
-        <v>55.834866</v>
+        <v>30.299465</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="n">
-        <v>37.50107</v>
+        <v>59.916189</v>
       </c>
       <c r="B114" t="n">
-        <v>55.827651</v>
+        <v>30.339296</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="n">
-        <v>37.46114</v>
+        <v>59.924366</v>
       </c>
       <c r="B115" t="n">
-        <v>55.8375</v>
+        <v>30.296348</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="n">
-        <v>37.495464</v>
+        <v>59.91683</v>
       </c>
       <c r="B116" t="n">
-        <v>55.800651</v>
+        <v>29.642042</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="n">
-        <v>37.495994</v>
+        <v>59.924366</v>
       </c>
       <c r="B117" t="n">
-        <v>55.804228</v>
+        <v>30.296348</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="n">
-        <v>37.276563</v>
+        <v>59.914191</v>
       </c>
       <c r="B118" t="n">
-        <v>55.898664</v>
+        <v>30.337176</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="n">
-        <v>37.667662</v>
+        <v>59.900421</v>
       </c>
       <c r="B119" t="n">
-        <v>55.622324</v>
+        <v>30.268186</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="n">
+        <v>59.92405</v>
+      </c>
+      <c r="B120" t="n">
+        <v>30.292602</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="n">
+        <v>59.853731</v>
+      </c>
+      <c r="B121" t="n">
+        <v>30.039079</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="n">
+        <v>59.909617</v>
+      </c>
+      <c r="B122" t="n">
+        <v>30.27477</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="n">
+        <v>59.997352</v>
+      </c>
+      <c r="B123" t="n">
+        <v>30.362419</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="n">
+        <v>59.836201</v>
+      </c>
+      <c r="B124" t="n">
+        <v>30.215275</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="n">
+        <v>59.939099</v>
+      </c>
+      <c r="B125" t="n">
+        <v>30.315877</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="n">
+        <v>59.972348</v>
+      </c>
+      <c r="B126" t="n">
+        <v>30.38591</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="n">
+        <v>59.941502</v>
+      </c>
+      <c r="B127" t="n">
+        <v>30.393501</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="n">
+        <v>59.858539</v>
+      </c>
+      <c r="B128" t="n">
+        <v>30.327681</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="n">
+        <v>60.042999</v>
+      </c>
+      <c r="B129" t="n">
+        <v>30.392081</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="n">
+        <v>59.930273</v>
+      </c>
+      <c r="B130" t="n">
+        <v>30.370207</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="n">
+        <v>59.934997</v>
+      </c>
+      <c r="B131" t="n">
+        <v>30.380304</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="n">
+        <v>59.92235</v>
+      </c>
+      <c r="B132" t="n">
+        <v>30.327897</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="n">
+        <v>59.747806</v>
+      </c>
+      <c r="B133" t="n">
+        <v>30.605233</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="n">
+        <v>59.871924</v>
+      </c>
+      <c r="B134" t="n">
+        <v>29.913576</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="n">
+        <v>59.943372</v>
+      </c>
+      <c r="B135" t="n">
+        <v>30.281238</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="n">
+        <v>59.995476</v>
+      </c>
+      <c r="B136" t="n">
+        <v>30.202348</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="n">
+        <v>59.867552</v>
+      </c>
+      <c r="B137" t="n">
+        <v>30.460632</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="n">
+        <v>59.919364</v>
+      </c>
+      <c r="B138" t="n">
+        <v>30.440698</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="n">
+        <v>59.918354</v>
+      </c>
+      <c r="B139" t="n">
+        <v>30.349824</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="n">
+        <v>59.811093</v>
+      </c>
+      <c r="B140" t="n">
+        <v>30.569714</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="n">
+        <v>59.837074</v>
+      </c>
+      <c r="B141" t="n">
+        <v>30.141927</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="n">
+        <v>59.924582</v>
+      </c>
+      <c r="B142" t="n">
+        <v>30.323342</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="n">
+        <v>59.924645</v>
+      </c>
+      <c r="B143" t="n">
+        <v>30.303382</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="n">
+        <v>59.902686</v>
+      </c>
+      <c r="B144" t="n">
+        <v>30.337275</v>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="n">
+        <v>59.925525</v>
+      </c>
+      <c r="B145" t="n">
+        <v>30.349294</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="n">
+        <v>60.092137</v>
+      </c>
+      <c r="B146" t="n">
+        <v>29.966774</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="n">
+        <v>59.940627</v>
+      </c>
+      <c r="B147" t="n">
+        <v>30.348827</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="n">
+        <v>59.732838</v>
+      </c>
+      <c r="B148" t="n">
+        <v>30.083636</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="n">
+        <v>59.983374</v>
+      </c>
+      <c r="B149" t="n">
+        <v>30.34704</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="n">
+        <v>59.928708</v>
+      </c>
+      <c r="B150" t="n">
+        <v>30.242754</v>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="n">
+        <v>59.841794</v>
+      </c>
+      <c r="B151" t="n">
+        <v>30.424187</v>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="n">
+        <v>60.013204</v>
+      </c>
+      <c r="B152" t="n">
+        <v>30.320503</v>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="n">
+        <v>59.785975</v>
+      </c>
+      <c r="B153" t="n">
+        <v>30.623388</v>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="n">
+        <v>59.917804</v>
+      </c>
+      <c r="B154" t="n">
+        <v>30.278202</v>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="n">
+        <v>59.907316</v>
+      </c>
+      <c r="B155" t="n">
+        <v>30.295575</v>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="n">
+        <v>59.918566</v>
+      </c>
+      <c r="B156" t="n">
+        <v>30.299043</v>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="n">
+        <v>59.802372</v>
+      </c>
+      <c r="B157" t="n">
+        <v>30.513515</v>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="n">
+        <v>60.20313</v>
+      </c>
+      <c r="B158" t="n">
+        <v>29.69418</v>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="n">
+        <v>59.886293</v>
+      </c>
+      <c r="B159" t="n">
+        <v>30.479092</v>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="n">
+        <v>59.859926</v>
+      </c>
+      <c r="B160" t="n">
+        <v>29.992816</v>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="n">
+        <v>59.860328</v>
+      </c>
+      <c r="B161" t="n">
+        <v>30.328238</v>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="n">
+        <v>60.019019</v>
+      </c>
+      <c r="B162" t="n">
+        <v>30.283475</v>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="n">
+        <v>59.900809</v>
+      </c>
+      <c r="B163" t="n">
+        <v>29.712488</v>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="n">
+        <v>59.95229</v>
+      </c>
+      <c r="B164" t="n">
+        <v>30.213846</v>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="n">
+        <v>59.84145</v>
+      </c>
+      <c r="B165" t="n">
+        <v>29.898789</v>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="n">
+        <v>59.933059</v>
+      </c>
+      <c r="B166" t="n">
+        <v>30.27486</v>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="n">
+        <v>59.954043</v>
+      </c>
+      <c r="B167" t="n">
+        <v>30.217745</v>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="n">
+        <v>59.954773</v>
+      </c>
+      <c r="B168" t="n">
+        <v>30.214745</v>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="n">
+        <v>59.943543</v>
+      </c>
+      <c r="B169" t="n">
+        <v>30.27088</v>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" t="n">
+        <v>59.945639</v>
+      </c>
+      <c r="B170" t="n">
+        <v>30.216434</v>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" t="n">
+        <v>59.945639</v>
+      </c>
+      <c r="B171" t="n">
+        <v>30.267916</v>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" t="n">
+        <v>59.936169</v>
+      </c>
+      <c r="B172" t="n">
+        <v>30.236044</v>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" t="n">
+        <v>59.947338</v>
+      </c>
+      <c r="B173" t="n">
+        <v>30.260577</v>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="n">
+        <v>60.050475</v>
+      </c>
+      <c r="B174" t="n">
+        <v>30.311143</v>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" t="n">
+        <v>60.043952</v>
+      </c>
+      <c r="B175" t="n">
+        <v>30.324079</v>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" t="n">
+        <v>59.911701</v>
+      </c>
+      <c r="B176" t="n">
+        <v>30.279091</v>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" t="n">
+        <v>59.973987</v>
+      </c>
+      <c r="B177" t="n">
+        <v>30.306445</v>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" t="n">
+        <v>60.048494</v>
+      </c>
+      <c r="B178" t="n">
+        <v>30.367261</v>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" t="n">
+        <v>60.052816</v>
+      </c>
+      <c r="B179" t="n">
+        <v>30.355098</v>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" t="n">
+        <v>60.047236</v>
+      </c>
+      <c r="B180" t="n">
+        <v>30.451109</v>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" t="n">
+        <v>60.030146</v>
+      </c>
+      <c r="B181" t="n">
+        <v>30.309248</v>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" t="n">
+        <v>59.981321</v>
+      </c>
+      <c r="B182" t="n">
+        <v>30.353813</v>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" t="n">
+        <v>60.037063</v>
+      </c>
+      <c r="B183" t="n">
+        <v>30.33149</v>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" t="n">
+        <v>60.088987</v>
+      </c>
+      <c r="B184" t="n">
+        <v>30.275031</v>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" t="n">
+        <v>60.075488</v>
+      </c>
+      <c r="B185" t="n">
+        <v>30.293249</v>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" t="n">
+        <v>60.034843</v>
+      </c>
+      <c r="B186" t="n">
+        <v>30.393518</v>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" t="n">
+        <v>60.000353</v>
+      </c>
+      <c r="B187" t="n">
+        <v>30.435093</v>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" t="n">
+        <v>59.997793</v>
+      </c>
+      <c r="B188" t="n">
+        <v>30.448909</v>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" t="n">
+        <v>60.013312</v>
+      </c>
+      <c r="B189" t="n">
+        <v>30.36055</v>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" t="n">
+        <v>59.974671</v>
+      </c>
+      <c r="B190" t="n">
+        <v>30.387688</v>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" t="n">
+        <v>60.128144</v>
+      </c>
+      <c r="B191" t="n">
+        <v>30.439701</v>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" t="n">
+        <v>59.97893</v>
+      </c>
+      <c r="B192" t="n">
+        <v>30.353472</v>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" t="n">
+        <v>60.020071</v>
+      </c>
+      <c r="B193" t="n">
+        <v>30.411494</v>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" t="n">
+        <v>60.00895</v>
+      </c>
+      <c r="B194" t="n">
+        <v>30.344255</v>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" t="n">
+        <v>59.89292</v>
+      </c>
+      <c r="B195" t="n">
+        <v>30.266542</v>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" t="n">
+        <v>59.876865</v>
+      </c>
+      <c r="B196" t="n">
+        <v>30.263999</v>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" t="n">
+        <v>59.868401</v>
+      </c>
+      <c r="B197" t="n">
+        <v>30.248764</v>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" t="n">
+        <v>59.778679</v>
+      </c>
+      <c r="B198" t="n">
+        <v>30.130743</v>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" t="n">
+        <v>59.868699</v>
+      </c>
+      <c r="B199" t="n">
+        <v>30.238631</v>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200" t="n">
+        <v>59.882939</v>
+      </c>
+      <c r="B200" t="n">
+        <v>30.267916</v>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" t="n">
+        <v>59.867145</v>
+      </c>
+      <c r="B201" t="n">
+        <v>30.259454</v>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202" t="n">
+        <v>59.846554</v>
+      </c>
+      <c r="B202" t="n">
+        <v>30.244362</v>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203" t="n">
+        <v>59.905317</v>
+      </c>
+      <c r="B203" t="n">
+        <v>30.270638</v>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204" t="n">
+        <v>59.935967</v>
+      </c>
+      <c r="B204" t="n">
+        <v>30.406589</v>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" t="n">
+        <v>59.963052</v>
+      </c>
+      <c r="B205" t="n">
+        <v>30.416749</v>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" t="n">
+        <v>60.047236</v>
+      </c>
+      <c r="B206" t="n">
+        <v>30.451109</v>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207" t="n">
+        <v>59.958336</v>
+      </c>
+      <c r="B207" t="n">
+        <v>30.410434</v>
+      </c>
+    </row>
+    <row r="208">
+      <c r="A208" t="n">
+        <v>59.92309</v>
+      </c>
+      <c r="B208" t="n">
+        <v>30.408655</v>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" t="n">
+        <v>59.984436</v>
+      </c>
+      <c r="B209" t="n">
+        <v>30.507667</v>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210" t="n">
+        <v>59.973208</v>
+      </c>
+      <c r="B210" t="n">
+        <v>30.416956</v>
+      </c>
+    </row>
+    <row r="211">
+      <c r="A211" t="n">
+        <v>59.954858</v>
+      </c>
+      <c r="B211" t="n">
+        <v>30.441677</v>
+      </c>
+    </row>
+    <row r="212">
+      <c r="A212" t="n">
+        <v>59.938635</v>
+      </c>
+      <c r="B212" t="n">
+        <v>30.487608</v>
+      </c>
+    </row>
+    <row r="213">
+      <c r="A213" t="n">
+        <v>59.961674</v>
+      </c>
+      <c r="B213" t="n">
+        <v>30.455664</v>
+      </c>
+    </row>
+    <row r="214">
+      <c r="A214" t="n">
+        <v>59.921962</v>
+      </c>
+      <c r="B214" t="n">
+        <v>30.416875</v>
+      </c>
+    </row>
+    <row r="215">
+      <c r="A215" t="n">
+        <v>59.952254</v>
+      </c>
+      <c r="B215" t="n">
+        <v>30.408395</v>
+      </c>
+    </row>
+    <row r="216">
+      <c r="A216" t="n">
+        <v>59.95457</v>
+      </c>
+      <c r="B216" t="n">
+        <v>30.436215</v>
+      </c>
+    </row>
+    <row r="217">
+      <c r="A217" t="n">
+        <v>59.940114</v>
+      </c>
+      <c r="B217" t="n">
+        <v>30.481104</v>
+      </c>
+    </row>
+    <row r="218">
+      <c r="A218" t="n">
+        <v>59.955597</v>
+      </c>
+      <c r="B218" t="n">
+        <v>30.491489</v>
+      </c>
+    </row>
+    <row r="219">
+      <c r="A219" t="n">
+        <v>59.828903</v>
+      </c>
+      <c r="B219" t="n">
+        <v>30.094604</v>
+      </c>
+    </row>
+    <row r="220">
+      <c r="A220" t="n">
+        <v>59.851096</v>
+      </c>
+      <c r="B220" t="n">
+        <v>30.060962</v>
+      </c>
+    </row>
+    <row r="221">
+      <c r="A221" t="n">
+        <v>59.868248</v>
+      </c>
+      <c r="B221" t="n">
+        <v>29.977958</v>
+      </c>
+    </row>
+    <row r="222">
+      <c r="A222" t="n">
+        <v>59.709853</v>
+      </c>
+      <c r="B222" t="n">
+        <v>30.340365</v>
+      </c>
+    </row>
+    <row r="223">
+      <c r="A223" t="n">
+        <v>59.818807</v>
+      </c>
+      <c r="B223" t="n">
+        <v>30.191209</v>
+      </c>
+    </row>
+    <row r="224">
+      <c r="A224" t="n">
+        <v>59.866364</v>
+      </c>
+      <c r="B224" t="n">
+        <v>30.355906</v>
+      </c>
+    </row>
+    <row r="225">
+      <c r="A225" t="n">
+        <v>59.885426</v>
+      </c>
+      <c r="B225" t="n">
+        <v>30.320072</v>
+      </c>
+    </row>
+    <row r="226">
+      <c r="A226" t="n">
+        <v>59.873419</v>
+      </c>
+      <c r="B226" t="n">
+        <v>30.308044</v>
+      </c>
+    </row>
+    <row r="227">
+      <c r="A227" t="n">
+        <v>59.85139</v>
+      </c>
+      <c r="B227" t="n">
+        <v>30.339754</v>
+      </c>
+    </row>
+    <row r="228">
+      <c r="A228" t="n">
+        <v>59.889372</v>
+      </c>
+      <c r="B228" t="n">
+        <v>30.323333</v>
+      </c>
+    </row>
+    <row r="229">
+      <c r="A229" t="n">
+        <v>59.873329</v>
+      </c>
+      <c r="B229" t="n">
+        <v>30.291155</v>
+      </c>
+    </row>
+    <row r="230">
+      <c r="A230" t="n">
+        <v>59.899338</v>
+      </c>
+      <c r="B230" t="n">
+        <v>30.340248</v>
+      </c>
+    </row>
+    <row r="231">
+      <c r="A231" t="n">
+        <v>59.897691</v>
+      </c>
+      <c r="B231" t="n">
+        <v>30.338398</v>
+      </c>
+    </row>
+    <row r="232">
+      <c r="A232" t="n">
+        <v>59.858801</v>
+      </c>
+      <c r="B232" t="n">
+        <v>30.327906</v>
+      </c>
+    </row>
+    <row r="233">
+      <c r="A233" t="n">
+        <v>59.885426</v>
+      </c>
+      <c r="B233" t="n">
+        <v>30.320072</v>
+      </c>
+    </row>
+    <row r="234">
+      <c r="A234" t="n">
+        <v>59.888862</v>
+      </c>
+      <c r="B234" t="n">
+        <v>30.315823</v>
+      </c>
+    </row>
+    <row r="235">
+      <c r="A235" t="n">
+        <v>59.856786</v>
+      </c>
+      <c r="B235" t="n">
+        <v>30.361305</v>
+      </c>
+    </row>
+    <row r="236">
+      <c r="A236" t="n">
+        <v>59.858363</v>
+      </c>
+      <c r="B236" t="n">
+        <v>30.319875</v>
+      </c>
+    </row>
+    <row r="237">
+      <c r="A237" t="n">
+        <v>59.843091</v>
+      </c>
+      <c r="B237" t="n">
+        <v>30.321977</v>
+      </c>
+    </row>
+    <row r="238">
+      <c r="A238" t="n">
+        <v>59.888212</v>
+      </c>
+      <c r="B238" t="n">
+        <v>30.331948</v>
+      </c>
+    </row>
+    <row r="239">
+      <c r="A239" t="n">
+        <v>59.840709</v>
+      </c>
+      <c r="B239" t="n">
+        <v>30.339826</v>
+      </c>
+    </row>
+    <row r="240">
+      <c r="A240" t="n">
+        <v>59.860328</v>
+      </c>
+      <c r="B240" t="n">
+        <v>30.328238</v>
+      </c>
+    </row>
+    <row r="241">
+      <c r="A241" t="n">
+        <v>59.892852</v>
+      </c>
+      <c r="B241" t="n">
+        <v>30.436575</v>
+      </c>
+    </row>
+    <row r="242">
+      <c r="A242" t="n">
+        <v>59.899058</v>
+      </c>
+      <c r="B242" t="n">
+        <v>30.427933</v>
+      </c>
+    </row>
+    <row r="243">
+      <c r="A243" t="n">
+        <v>59.884243</v>
+      </c>
+      <c r="B243" t="n">
+        <v>30.438416</v>
+      </c>
+    </row>
+    <row r="244">
+      <c r="A244" t="n">
+        <v>59.944711</v>
+      </c>
+      <c r="B244" t="n">
+        <v>30.494462</v>
+      </c>
+    </row>
+    <row r="245">
+      <c r="A245" t="n">
+        <v>59.906639</v>
+      </c>
+      <c r="B245" t="n">
+        <v>30.404667</v>
+      </c>
+    </row>
+    <row r="246">
+      <c r="A246" t="n">
+        <v>59.945639</v>
+      </c>
+      <c r="B246" t="n">
+        <v>30.267916</v>
+      </c>
+    </row>
+    <row r="247">
+      <c r="A247" t="n">
+        <v>59.922269</v>
+      </c>
+      <c r="B247" t="n">
+        <v>30.444183</v>
+      </c>
+    </row>
+    <row r="248">
+      <c r="A248" t="n">
+        <v>59.861196</v>
+      </c>
+      <c r="B248" t="n">
+        <v>30.476065</v>
+      </c>
+    </row>
+    <row r="249">
+      <c r="A249" t="n">
+        <v>59.943214</v>
+      </c>
+      <c r="B249" t="n">
+        <v>30.479442</v>
+      </c>
+    </row>
+    <row r="250">
+      <c r="A250" t="n">
+        <v>59.865</v>
+      </c>
+      <c r="B250" t="n">
+        <v>30.44598</v>
+      </c>
+    </row>
+    <row r="251">
+      <c r="A251" t="n">
+        <v>59.966349</v>
+      </c>
+      <c r="B251" t="n">
+        <v>30.474106</v>
+      </c>
+    </row>
+    <row r="252">
+      <c r="A252" t="n">
+        <v>59.899712</v>
+      </c>
+      <c r="B252" t="n">
+        <v>30.423423</v>
+      </c>
+    </row>
+    <row r="253">
+      <c r="A253" t="n">
+        <v>59.865587</v>
+      </c>
+      <c r="B253" t="n">
+        <v>30.466013</v>
+      </c>
+    </row>
+    <row r="254">
+      <c r="A254" t="n">
+        <v>59.882171</v>
+      </c>
+      <c r="B254" t="n">
+        <v>30.489369</v>
+      </c>
+    </row>
+    <row r="255">
+      <c r="A255" t="n">
+        <v>59.899329</v>
+      </c>
+      <c r="B255" t="n">
+        <v>30.493609</v>
+      </c>
+    </row>
+    <row r="256">
+      <c r="A256" t="n">
+        <v>59.968232</v>
+      </c>
+      <c r="B256" t="n">
+        <v>30.308843</v>
+      </c>
+    </row>
+    <row r="257">
+      <c r="A257" t="n">
+        <v>59.962836</v>
+      </c>
+      <c r="B257" t="n">
+        <v>30.30136</v>
+      </c>
+    </row>
+    <row r="258">
+      <c r="A258" t="n">
+        <v>59.958246</v>
+      </c>
+      <c r="B258" t="n">
+        <v>30.263344</v>
+      </c>
+    </row>
+    <row r="259">
+      <c r="A259" t="n">
+        <v>59.968025</v>
+      </c>
+      <c r="B259" t="n">
+        <v>30.263281</v>
+      </c>
+    </row>
+    <row r="260">
+      <c r="A260" t="n">
+        <v>59.958683</v>
+      </c>
+      <c r="B260" t="n">
+        <v>30.304765</v>
+      </c>
+    </row>
+    <row r="261">
+      <c r="A261" t="n">
+        <v>60.026963</v>
+      </c>
+      <c r="B261" t="n">
+        <v>30.298638</v>
+      </c>
+    </row>
+    <row r="262">
+      <c r="A262" t="n">
+        <v>59.991894</v>
+      </c>
+      <c r="B262" t="n">
+        <v>30.321177</v>
+      </c>
+    </row>
+    <row r="263">
+      <c r="A263" t="n">
+        <v>59.995476</v>
+      </c>
+      <c r="B263" t="n">
+        <v>30.202348</v>
+      </c>
+    </row>
+    <row r="264">
+      <c r="A264" t="n">
+        <v>59.995476</v>
+      </c>
+      <c r="B264" t="n">
+        <v>30.202348</v>
+      </c>
+    </row>
+    <row r="265">
+      <c r="A265" t="n">
+        <v>60.017976</v>
+      </c>
+      <c r="B265" t="n">
+        <v>30.277699</v>
+      </c>
+    </row>
+    <row r="266">
+      <c r="A266" t="n">
+        <v>59.998256</v>
+      </c>
+      <c r="B266" t="n">
+        <v>30.293096</v>
+      </c>
+    </row>
+    <row r="267">
+      <c r="A267" t="n">
+        <v>59.938955</v>
+      </c>
+      <c r="B267" t="n">
+        <v>30.315644</v>
+      </c>
+    </row>
+    <row r="268">
+      <c r="A268" t="n">
+        <v>60.017535</v>
+      </c>
+      <c r="B268" t="n">
+        <v>30.283035</v>
+      </c>
+    </row>
+    <row r="269">
+      <c r="A269" t="n">
+        <v>59.942403</v>
+      </c>
+      <c r="B269" t="n">
+        <v>30.352052</v>
+      </c>
+    </row>
+    <row r="270">
+      <c r="A270" t="n">
+        <v>60.033616</v>
+      </c>
+      <c r="B270" t="n">
+        <v>30.244407</v>
+      </c>
+    </row>
+    <row r="271">
+      <c r="A271" t="n">
+        <v>59.995017</v>
+      </c>
+      <c r="B271" t="n">
+        <v>30.148781</v>
+      </c>
+    </row>
+    <row r="272">
+      <c r="A272" t="n">
+        <v>59.910496</v>
+      </c>
+      <c r="B272" t="n">
+        <v>30.254298</v>
+      </c>
+    </row>
+    <row r="273">
+      <c r="A273" t="n">
+        <v>59.997982</v>
+      </c>
+      <c r="B273" t="n">
+        <v>30.271617</v>
+      </c>
+    </row>
+    <row r="274">
+      <c r="A274" t="n">
+        <v>59.983504</v>
+      </c>
+      <c r="B274" t="n">
+        <v>30.219605</v>
+      </c>
+    </row>
+    <row r="275">
+      <c r="A275" t="n">
+        <v>59.864286</v>
+      </c>
+      <c r="B275" t="n">
+        <v>30.399088</v>
+      </c>
+    </row>
+    <row r="276">
+      <c r="A276" t="n">
+        <v>59.862976</v>
+      </c>
+      <c r="B276" t="n">
+        <v>30.415563</v>
+      </c>
+    </row>
+    <row r="277">
+      <c r="A277" t="n">
+        <v>60.016645</v>
+      </c>
+      <c r="B277" t="n">
+        <v>30.292871</v>
+      </c>
+    </row>
+    <row r="278">
+      <c r="A278" t="n">
+        <v>59.841794</v>
+      </c>
+      <c r="B278" t="n">
+        <v>30.424187</v>
+      </c>
+    </row>
+    <row r="279">
+      <c r="A279" t="n">
+        <v>59.884085</v>
+      </c>
+      <c r="B279" t="n">
+        <v>30.390761</v>
+      </c>
+    </row>
+    <row r="280">
+      <c r="A280" t="n">
+        <v>59.939591</v>
+      </c>
+      <c r="B280" t="n">
+        <v>30.361296</v>
+      </c>
+    </row>
+    <row r="281">
+      <c r="A281" t="n">
+        <v>59.850477</v>
+      </c>
+      <c r="B281" t="n">
+        <v>30.368698</v>
+      </c>
+    </row>
+    <row r="282">
+      <c r="A282" t="n">
+        <v>59.857111</v>
+      </c>
+      <c r="B282" t="n">
+        <v>30.365725</v>
+      </c>
+    </row>
+    <row r="283">
+      <c r="A283" t="n">
+        <v>59.905782</v>
+      </c>
+      <c r="B283" t="n">
+        <v>30.364656</v>
+      </c>
+    </row>
+    <row r="284">
+      <c r="A284" t="n">
+        <v>59.839086</v>
+      </c>
+      <c r="B284" t="n">
+        <v>30.38494</v>
+      </c>
+    </row>
+    <row r="285">
+      <c r="A285" t="n">
+        <v>59.942025</v>
+      </c>
+      <c r="B285" t="n">
+        <v>30.344956</v>
+      </c>
+    </row>
+    <row r="286">
+      <c r="A286" t="n">
+        <v>59.944368</v>
+      </c>
+      <c r="B286" t="n">
+        <v>30.345566</v>
+      </c>
+    </row>
+    <row r="287">
+      <c r="A287" t="n">
+        <v>59.939523</v>
+      </c>
+      <c r="B287" t="n">
+        <v>30.358484</v>
+      </c>
+    </row>
+    <row r="288">
+      <c r="A288" t="n">
+        <v>59.949195</v>
+      </c>
+      <c r="B288" t="n">
+        <v>30.35269</v>
+      </c>
+    </row>
+    <row r="289">
+      <c r="A289" t="n">
+        <v>59.937418</v>
+      </c>
+      <c r="B289" t="n">
+        <v>30.378023</v>
+      </c>
+    </row>
+    <row r="290">
+      <c r="A290" t="n">
+        <v>59.926449</v>
+      </c>
+      <c r="B290" t="n">
+        <v>30.333134</v>
+      </c>
+    </row>
+    <row r="291">
+      <c r="A291" t="n">
+        <v>59.924938</v>
+      </c>
+      <c r="B291" t="n">
+        <v>30.344722</v>
+      </c>
+    </row>
+    <row r="292">
+      <c r="A292" t="n">
+        <v>59.934344</v>
+      </c>
+      <c r="B292" t="n">
+        <v>30.392566</v>
+      </c>
+    </row>
+    <row r="293">
+      <c r="A293" t="n">
+        <v>59.941615</v>
+      </c>
+      <c r="B293" t="n">
+        <v>30.351693</v>
+      </c>
+    </row>
+    <row r="294">
+      <c r="A294" t="n">
+        <v>59.939613</v>
+      </c>
+      <c r="B294" t="n">
+        <v>30.37725</v>
+      </c>
+    </row>
+    <row r="295">
+      <c r="A295" t="n">
+        <v>59.836893</v>
+      </c>
+      <c r="B295" t="n">
+        <v>29.90541</v>
+      </c>
+    </row>
+    <row r="296">
+      <c r="A296" t="n">
+        <v>59.927915</v>
+      </c>
+      <c r="B296" t="n">
+        <v>30.338425</v>
+      </c>
+    </row>
+    <row r="297">
+      <c r="A297" t="n">
+        <v>59.91724</v>
+      </c>
+      <c r="B297" t="n">
+        <v>30.345279</v>
+      </c>
+    </row>
+    <row r="298">
+      <c r="A298" t="n">
+        <v>59.947554</v>
+      </c>
+      <c r="B298" t="n">
+        <v>30.360398</v>
+      </c>
+    </row>
+    <row r="299">
+      <c r="A299" t="n">
+        <v>59.92157</v>
+      </c>
+      <c r="B299" t="n">
+        <v>30.345611</v>
+      </c>
+    </row>
+    <row r="300">
+      <c r="A300" t="n">
+        <v>59.912098</v>
+      </c>
+      <c r="B300" t="n">
+        <v>30.354262</v>
+      </c>
+    </row>
+    <row r="301">
+      <c r="A301" t="n">
+        <v>60.033926</v>
+      </c>
+      <c r="B301" t="n">
+        <v>30.313532</v>
+      </c>
+    </row>
+    <row r="302">
+      <c r="A302" t="n">
+        <v>59.842725</v>
+      </c>
+      <c r="B302" t="n">
+        <v>30.31841</v>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="n">
+        <v>60.039099</v>
+      </c>
+      <c r="B303" t="n">
+        <v>30.299106</v>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="n">
+        <v>59.841844</v>
+      </c>
+      <c r="B304" t="n">
+        <v>30.349375</v>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="n">
+        <v>60.047236</v>
+      </c>
+      <c r="B305" t="n">
+        <v>30.451109</v>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="n">
+        <v>60.047236</v>
+      </c>
+      <c r="B306" t="n">
+        <v>30.451109</v>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="n">
+        <v>59.890947</v>
+      </c>
+      <c r="B307" t="n">
+        <v>30.266883</v>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="n">
+        <v>59.810242</v>
+      </c>
+      <c r="B308" t="n">
+        <v>30.174392</v>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="n">
+        <v>59.929939</v>
+      </c>
+      <c r="B309" t="n">
+        <v>30.350049</v>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="n">
+        <v>60.055493</v>
+      </c>
+      <c r="B310" t="n">
+        <v>29.976053</v>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="n">
+        <v>59.92855</v>
+      </c>
+      <c r="B311" t="n">
+        <v>30.24756</v>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="n">
+        <v>59.901247</v>
+      </c>
+      <c r="B312" t="n">
+        <v>30.487698</v>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="n">
+        <v>59.882324</v>
+      </c>
+      <c r="B313" t="n">
+        <v>29.890363</v>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="n">
+        <v>59.990579</v>
+      </c>
+      <c r="B314" t="n">
+        <v>30.262059</v>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="n">
+        <v>59.874575</v>
+      </c>
+      <c r="B315" t="n">
+        <v>30.443752</v>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="n">
+        <v>59.960179</v>
+      </c>
+      <c r="B316" t="n">
+        <v>30.22883</v>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="n">
+        <v>59.941615</v>
+      </c>
+      <c r="B317" t="n">
+        <v>30.351693</v>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="n">
+        <v>59.819115</v>
+      </c>
+      <c r="B318" t="n">
+        <v>29.981156</v>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="n">
+        <v>59.843335</v>
+      </c>
+      <c r="B319" t="n">
+        <v>30.021858</v>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="n">
+        <v>59.873451</v>
+      </c>
+      <c r="B320" t="n">
+        <v>30.384014</v>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="n">
+        <v>59.940402</v>
+      </c>
+      <c r="B321" t="n">
+        <v>30.264287</v>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="n">
+        <v>60.150415</v>
+      </c>
+      <c r="B322" t="n">
+        <v>29.927877</v>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="n">
+        <v>59.727921</v>
+      </c>
+      <c r="B323" t="n">
+        <v>30.09597</v>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="n">
+        <v>59.85139</v>
+      </c>
+      <c r="B324" t="n">
+        <v>30.339458</v>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="n">
+        <v>59.877958</v>
+      </c>
+      <c r="B325" t="n">
+        <v>30.482012</v>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="n">
+        <v>59.813346</v>
+      </c>
+      <c r="B326" t="n">
+        <v>30.056066</v>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="n">
+        <v>59.940889</v>
+      </c>
+      <c r="B327" t="n">
+        <v>30.289494</v>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="n">
+        <v>60.084733</v>
+      </c>
+      <c r="B328" t="n">
+        <v>30.267395</v>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="n">
+        <v>60.015709</v>
+      </c>
+      <c r="B329" t="n">
+        <v>30.294039</v>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="n">
+        <v>59.945603</v>
+      </c>
+      <c r="B330" t="n">
+        <v>30.706204</v>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="n">
+        <v>59.917804</v>
+      </c>
+      <c r="B331" t="n">
+        <v>30.278202</v>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="n">
+        <v>59.929687</v>
+      </c>
+      <c r="B332" t="n">
+        <v>30.472355</v>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="n">
+        <v>59.987046</v>
+      </c>
+      <c r="B333" t="n">
+        <v>30.314691</v>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="n">
+        <v>60.066096</v>
+      </c>
+      <c r="B334" t="n">
+        <v>30.302402</v>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" t="n">
+        <v>59.953493</v>
+      </c>
+      <c r="B335" t="n">
+        <v>30.221823</v>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" t="n">
+        <v>60.286924</v>
+      </c>
+      <c r="B336" t="n">
+        <v>29.745977</v>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" t="n">
+        <v>59.954264</v>
+      </c>
+      <c r="B337" t="n">
+        <v>30.41435</v>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" t="n">
+        <v>59.910875</v>
+      </c>
+      <c r="B338" t="n">
+        <v>30.318015</v>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" t="n">
+        <v>59.9583</v>
+      </c>
+      <c r="B339" t="n">
+        <v>30.30225</v>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" t="n">
+        <v>59.959899</v>
+      </c>
+      <c r="B340" t="n">
+        <v>30.288443</v>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" t="n">
+        <v>60.085245</v>
+      </c>
+      <c r="B341" t="n">
+        <v>30.267197</v>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" t="n">
+        <v>60.010375</v>
+      </c>
+      <c r="B342" t="n">
+        <v>30.611351</v>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" t="n">
+        <v>60.041067</v>
+      </c>
+      <c r="B343" t="n">
+        <v>30.645981</v>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" t="n">
+        <v>60.01096</v>
+      </c>
+      <c r="B344" t="n">
+        <v>30.650221</v>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" t="n">
+        <v>60.141676</v>
+      </c>
+      <c r="B345" t="n">
+        <v>30.210819</v>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" t="n">
+        <v>60.149927</v>
+      </c>
+      <c r="B346" t="n">
+        <v>30.511979</v>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" t="n">
+        <v>60.042572</v>
+      </c>
+      <c r="B347" t="n">
+        <v>30.301585</v>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" t="n">
+        <v>60.123053</v>
+      </c>
+      <c r="B348" t="n">
+        <v>30.169793</v>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" t="n">
+        <v>59.950447</v>
+      </c>
+      <c r="B349" t="n">
+        <v>30.249474</v>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" t="n">
+        <v>60.531715</v>
+      </c>
+      <c r="B350" t="n">
+        <v>30.01699</v>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" t="n">
+        <v>59.922242</v>
+      </c>
+      <c r="B351" t="n">
+        <v>30.347399</v>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" t="n">
+        <v>59.940276</v>
+      </c>
+      <c r="B352" t="n">
+        <v>30.673568</v>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" t="n">
+        <v>59.987118</v>
+      </c>
+      <c r="B353" t="n">
+        <v>30.234157</v>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" t="n">
+        <v>59.839936</v>
+      </c>
+      <c r="B354" t="n">
+        <v>29.896633</v>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" t="n">
+        <v>59.88962</v>
+      </c>
+      <c r="B355" t="n">
+        <v>30.379136</v>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" t="n">
+        <v>59.903733</v>
+      </c>
+      <c r="B356" t="n">
+        <v>30.56498</v>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" t="n">
+        <v>60.047236</v>
+      </c>
+      <c r="B357" t="n">
+        <v>30.451109</v>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" t="n">
+        <v>59.919973</v>
+      </c>
+      <c r="B358" t="n">
+        <v>30.345629</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
v7 Add normal stars scrab
</commit_message>
<xml_diff>
--- a/Geocoding.xlsx
+++ b/Geocoding.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B358"/>
+  <dimension ref="A1:B426"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -423,2866 +423,3410 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="n">
-        <v>60.047236</v>
+        <v>55.801344</v>
       </c>
       <c r="B1" t="n">
-        <v>30.451109</v>
+        <v>37.31696</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>60.047236</v>
+        <v>55.766542</v>
       </c>
       <c r="B2" t="n">
-        <v>30.451109</v>
+        <v>37.678281</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>60.047236</v>
+        <v>55.80915</v>
       </c>
       <c r="B3" t="n">
-        <v>30.451109</v>
+        <v>37.533436</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>60.018839</v>
+        <v>55.827651</v>
       </c>
       <c r="B4" t="n">
-        <v>30.432685</v>
+        <v>37.50107</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>59.930629</v>
+        <v>55.791749</v>
       </c>
       <c r="B5" t="n">
-        <v>30.238505</v>
+        <v>37.748619</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>60.024131</v>
+        <v>55.796294</v>
       </c>
       <c r="B6" t="n">
-        <v>30.333843</v>
+        <v>37.620609</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>60.000267</v>
+        <v>55.714293</v>
       </c>
       <c r="B7" t="n">
-        <v>30.324366</v>
+        <v>37.69277</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>60.051284</v>
+        <v>55.907556</v>
       </c>
       <c r="B8" t="n">
-        <v>30.438578</v>
+        <v>37.554762</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>59.838186</v>
+        <v>55.768</v>
       </c>
       <c r="B9" t="n">
-        <v>30.231346</v>
+        <v>37.558634</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>59.909617</v>
+        <v>55.792609</v>
       </c>
       <c r="B10" t="n">
-        <v>30.278498</v>
+        <v>37.590659</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>59.839353</v>
+        <v>55.844581</v>
       </c>
       <c r="B11" t="n">
-        <v>30.239664</v>
+        <v>37.576672</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>59.856352</v>
+        <v>55.724226</v>
       </c>
       <c r="B12" t="n">
-        <v>30.197201</v>
+        <v>37.688027</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>59.91069</v>
+        <v>55.742777</v>
       </c>
       <c r="B13" t="n">
-        <v>30.31161</v>
+        <v>37.609667</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>60.05909</v>
+        <v>55.634629</v>
       </c>
       <c r="B14" t="n">
-        <v>30.335029</v>
+        <v>37.684677</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>60.077135</v>
+        <v>55.758792</v>
       </c>
       <c r="B15" t="n">
-        <v>30.252833</v>
+        <v>37.704071</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>59.859976</v>
+        <v>55.746274</v>
       </c>
       <c r="B16" t="n">
-        <v>30.178417</v>
+        <v>37.772092</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>59.83843</v>
+        <v>55.795641</v>
       </c>
       <c r="B17" t="n">
-        <v>30.204459</v>
+        <v>37.699292</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>59.930007</v>
+        <v>55.701699</v>
       </c>
       <c r="B18" t="n">
-        <v>30.315293</v>
+        <v>37.604044</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>59.901247</v>
+        <v>55.710393</v>
       </c>
       <c r="B19" t="n">
-        <v>30.487698</v>
+        <v>37.615398</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>59.942421</v>
+        <v>55.688624</v>
       </c>
       <c r="B20" t="n">
-        <v>30.283232</v>
+        <v>37.591404</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>59.937873</v>
+        <v>55.619808</v>
       </c>
       <c r="B21" t="n">
-        <v>30.305852</v>
+        <v>37.583329</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>59.93245</v>
+        <v>55.734004</v>
       </c>
       <c r="B22" t="n">
-        <v>30.349267</v>
+        <v>37.659452</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>59.904947</v>
+        <v>55.703677</v>
       </c>
       <c r="B23" t="n">
-        <v>30.273504</v>
+        <v>37.685701</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>59.9496</v>
+        <v>55.784784</v>
       </c>
       <c r="B24" t="n">
-        <v>30.305034</v>
+        <v>37.471309</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>59.922706</v>
+        <v>55.741247</v>
       </c>
       <c r="B25" t="n">
-        <v>30.458772</v>
+        <v>37.509002</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>60.044859</v>
+        <v>55.803044</v>
       </c>
       <c r="B26" t="n">
-        <v>30.351055</v>
+        <v>37.518596</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>60.081785</v>
+        <v>55.748179</v>
       </c>
       <c r="B27" t="n">
-        <v>30.248944</v>
+        <v>37.540245</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>59.909265</v>
+        <v>55.768451</v>
       </c>
       <c r="B28" t="n">
-        <v>30.312598</v>
+        <v>37.571911</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>59.901247</v>
+        <v>55.755864</v>
       </c>
       <c r="B29" t="n">
-        <v>30.487698</v>
+        <v>37.617698</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>59.930007</v>
+        <v>55.707015</v>
       </c>
       <c r="B30" t="n">
-        <v>30.315293</v>
+        <v>37.619432</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>59.920492</v>
+        <v>55.680311</v>
       </c>
       <c r="B31" t="n">
-        <v>30.359077</v>
+        <v>37.623492</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>59.90418</v>
+        <v>55.827788</v>
       </c>
       <c r="B32" t="n">
-        <v>30.457541</v>
+        <v>37.409163</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>60.072296</v>
+        <v>55.756123</v>
       </c>
       <c r="B33" t="n">
-        <v>30.362212</v>
+        <v>37.566737</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>59.977012</v>
+        <v>55.888922</v>
       </c>
       <c r="B34" t="n">
-        <v>30.331741</v>
+        <v>37.530571</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>59.979056</v>
+        <v>55.572279</v>
       </c>
       <c r="B35" t="n">
-        <v>30.337149</v>
+        <v>37.750613</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>60.051181</v>
+        <v>55.774836</v>
       </c>
       <c r="B36" t="n">
-        <v>30.333879</v>
+        <v>37.632664</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>60.028928</v>
+        <v>55.732306</v>
       </c>
       <c r="B37" t="n">
-        <v>30.330511</v>
+        <v>37.63031</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>60.00029</v>
+        <v>55.73443</v>
       </c>
       <c r="B38" t="n">
-        <v>30.316254</v>
+        <v>37.638413</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>59.943701</v>
+        <v>55.803737</v>
       </c>
       <c r="B39" t="n">
-        <v>30.371267</v>
+        <v>37.406289</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>59.842033</v>
+        <v>55.540608</v>
       </c>
       <c r="B40" t="n">
-        <v>30.131237</v>
+        <v>37.555041</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>59.967155</v>
+        <v>55.762596</v>
       </c>
       <c r="B41" t="n">
-        <v>30.273737</v>
+        <v>37.613539</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>59.968232</v>
+        <v>55.743578</v>
       </c>
       <c r="B42" t="n">
-        <v>30.308843</v>
+        <v>37.519036</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>59.833059</v>
+        <v>55.827788</v>
       </c>
       <c r="B43" t="n">
-        <v>30.173746</v>
+        <v>37.409163</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>59.854332</v>
+        <v>55.793202</v>
       </c>
       <c r="B44" t="n">
-        <v>30.387437</v>
+        <v>38.051369</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>59.965241</v>
+        <v>55.664187</v>
       </c>
       <c r="B45" t="n">
-        <v>30.406948</v>
+        <v>37.961349</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>60.041516</v>
+        <v>55.532197</v>
       </c>
       <c r="B46" t="n">
-        <v>30.318994</v>
+        <v>37.519494</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>60.084289</v>
+        <v>55.740983</v>
       </c>
       <c r="B47" t="n">
-        <v>30.267332</v>
+        <v>37.610323</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>59.84819</v>
+        <v>55.72563</v>
       </c>
       <c r="B48" t="n">
-        <v>30.40552</v>
+        <v>37.405076</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>59.952096</v>
+        <v>55.764678</v>
       </c>
       <c r="B49" t="n">
-        <v>30.436817</v>
+        <v>37.636805</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>60.047236</v>
+        <v>55.751817</v>
       </c>
       <c r="B50" t="n">
-        <v>30.451109</v>
+        <v>37.592752</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>60.047236</v>
+        <v>55.734785</v>
       </c>
       <c r="B51" t="n">
-        <v>30.451109</v>
+        <v>37.820331</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>60.018785</v>
+        <v>55.755819</v>
       </c>
       <c r="B52" t="n">
-        <v>30.280744</v>
+        <v>37.617644</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>59.938432</v>
+        <v>55.820561</v>
       </c>
       <c r="B53" t="n">
-        <v>30.212553</v>
+        <v>37.64798</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>59.929177</v>
+        <v>55.831514</v>
       </c>
       <c r="B54" t="n">
-        <v>30.364638</v>
+        <v>37.491287</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="n">
-        <v>59.938139</v>
+        <v>55.849676</v>
       </c>
       <c r="B55" t="n">
-        <v>30.47734</v>
+        <v>37.616692</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="n">
-        <v>60.013312</v>
+        <v>55.642337</v>
       </c>
       <c r="B56" t="n">
-        <v>30.36055</v>
+        <v>37.519961</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="n">
-        <v>59.928059</v>
+        <v>55.752024</v>
       </c>
       <c r="B57" t="n">
-        <v>30.305636</v>
+        <v>37.642069</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
-        <v>60.13621</v>
+        <v>55.820561</v>
       </c>
       <c r="B58" t="n">
-        <v>30.257846</v>
+        <v>37.660323</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="n">
-        <v>59.611928</v>
+        <v>55.639923</v>
       </c>
       <c r="B59" t="n">
-        <v>30.171554</v>
+        <v>37.593749</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="n">
-        <v>59.991358</v>
+        <v>55.66469</v>
       </c>
       <c r="B60" t="n">
-        <v>30.160981</v>
+        <v>37.578262</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="n">
-        <v>59.991358</v>
+        <v>55.662222</v>
       </c>
       <c r="B61" t="n">
-        <v>30.160981</v>
+        <v>37.620869</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="n">
-        <v>59.991358</v>
+        <v>55.882459</v>
       </c>
       <c r="B62" t="n">
-        <v>30.160981</v>
+        <v>37.71009</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="n">
-        <v>60.030542</v>
+        <v>55.733913</v>
       </c>
       <c r="B63" t="n">
-        <v>29.990705</v>
+        <v>37.56459</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="n">
-        <v>60.041332</v>
+        <v>55.661841</v>
       </c>
       <c r="B64" t="n">
-        <v>30.311799</v>
+        <v>38.011681</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="n">
-        <v>59.942885</v>
+        <v>55.67655</v>
       </c>
       <c r="B65" t="n">
-        <v>30.361116</v>
+        <v>37.678164</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="n">
-        <v>59.874697</v>
+        <v>55.771115</v>
       </c>
       <c r="B66" t="n">
-        <v>30.33591</v>
+        <v>37.67988</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="n">
-        <v>59.924406</v>
+        <v>55.551573</v>
       </c>
       <c r="B67" t="n">
-        <v>30.385784</v>
+        <v>38.257128</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="n">
-        <v>59.873586</v>
+        <v>55.724119</v>
       </c>
       <c r="B68" t="n">
-        <v>30.471142</v>
+        <v>37.689015</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="n">
-        <v>60.023362</v>
+        <v>55.755864</v>
       </c>
       <c r="B69" t="n">
-        <v>30.677018</v>
+        <v>37.617698</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="n">
-        <v>59.973028</v>
+        <v>55.80187</v>
       </c>
       <c r="B70" t="n">
-        <v>30.338461</v>
+        <v>37.632592</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="n">
-        <v>60.045565</v>
+        <v>55.755864</v>
       </c>
       <c r="B71" t="n">
-        <v>30.301208</v>
+        <v>37.617698</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="n">
-        <v>60.042173</v>
+        <v>55.772375</v>
       </c>
       <c r="B72" t="n">
-        <v>30.363865</v>
+        <v>37.683149</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="n">
-        <v>59.936377</v>
+        <v>55.683843</v>
       </c>
       <c r="B73" t="n">
-        <v>30.367701</v>
+        <v>37.440407</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="n">
-        <v>59.913663</v>
+        <v>55.659901</v>
       </c>
       <c r="B74" t="n">
-        <v>30.282639</v>
+        <v>37.628783</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="n">
-        <v>59.935791</v>
+        <v>55.811133</v>
       </c>
       <c r="B75" t="n">
-        <v>30.369273</v>
+        <v>37.497818</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="n">
-        <v>60.006498</v>
+        <v>55.735996</v>
       </c>
       <c r="B76" t="n">
-        <v>30.275642</v>
+        <v>37.736958</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="n">
-        <v>59.833059</v>
+        <v>55.677803</v>
       </c>
       <c r="B77" t="n">
-        <v>30.173746</v>
+        <v>37.449884</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="n">
-        <v>59.933911</v>
+        <v>55.791749</v>
       </c>
       <c r="B78" t="n">
-        <v>30.371195</v>
+        <v>37.748619</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="n">
-        <v>59.834926</v>
+        <v>55.682605</v>
       </c>
       <c r="B79" t="n">
-        <v>30.217206</v>
+        <v>37.86902</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="n">
-        <v>60.055753</v>
+        <v>55.832369</v>
       </c>
       <c r="B80" t="n">
-        <v>30.339332</v>
+        <v>37.454438</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="n">
-        <v>59.861828</v>
+        <v>55.832551</v>
       </c>
       <c r="B81" t="n">
-        <v>30.33829</v>
+        <v>37.448231</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="n">
-        <v>60.055672</v>
+        <v>55.785736</v>
       </c>
       <c r="B82" t="n">
-        <v>30.358502</v>
+        <v>37.596148</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="n">
-        <v>60.167975</v>
+        <v>55.888614</v>
       </c>
       <c r="B83" t="n">
-        <v>30.354954</v>
+        <v>37.600774</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="n">
-        <v>59.720608</v>
+        <v>55.573576</v>
       </c>
       <c r="B84" t="n">
-        <v>30.429244</v>
+        <v>37.583104</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="n">
-        <v>59.985638</v>
+        <v>55.744961</v>
       </c>
       <c r="B85" t="n">
-        <v>30.350399</v>
+        <v>37.508391</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="n">
-        <v>59.914556</v>
+        <v>55.733457</v>
       </c>
       <c r="B86" t="n">
-        <v>30.486467</v>
+        <v>37.709156</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="n">
-        <v>59.889634</v>
+        <v>55.824698</v>
       </c>
       <c r="B87" t="n">
-        <v>30.47664</v>
+        <v>37.710665</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="n">
-        <v>60.110298</v>
+        <v>55.722816</v>
       </c>
       <c r="B88" t="n">
-        <v>30.344776</v>
+        <v>37.78191</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="n">
-        <v>59.995417</v>
+        <v>55.657484</v>
       </c>
       <c r="B89" t="n">
-        <v>30.295063</v>
+        <v>37.731335</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="n">
-        <v>59.938955</v>
+        <v>55.736625</v>
       </c>
       <c r="B90" t="n">
-        <v>30.315644</v>
+        <v>37.58968</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="n">
-        <v>59.904184</v>
+        <v>55.654584</v>
       </c>
       <c r="B91" t="n">
-        <v>30.562824</v>
+        <v>37.702517</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="n">
-        <v>59.888952</v>
+        <v>55.763609</v>
       </c>
       <c r="B92" t="n">
-        <v>30.420468</v>
+        <v>37.608481</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="n">
-        <v>59.855331</v>
+        <v>55.667422</v>
       </c>
       <c r="B93" t="n">
-        <v>30.378678</v>
+        <v>37.5675</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="n">
-        <v>59.916582</v>
+        <v>55.780886</v>
       </c>
       <c r="B94" t="n">
-        <v>30.288227</v>
+        <v>37.560296</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="n">
-        <v>59.949104</v>
+        <v>55.755864</v>
       </c>
       <c r="B95" t="n">
-        <v>30.342997</v>
+        <v>37.617698</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="n">
-        <v>59.953637</v>
+        <v>55.810081</v>
       </c>
       <c r="B96" t="n">
-        <v>30.449322</v>
+        <v>37.795645</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="n">
-        <v>59.838055</v>
+        <v>55.733518</v>
       </c>
       <c r="B97" t="n">
-        <v>30.350444</v>
+        <v>37.663881</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="n">
-        <v>59.993784</v>
+        <v>55.81778</v>
       </c>
       <c r="B98" t="n">
-        <v>30.107594</v>
+        <v>37.808321</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="n">
-        <v>59.97106</v>
+        <v>55.809403</v>
       </c>
       <c r="B99" t="n">
-        <v>30.434787</v>
+        <v>37.783949</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="n">
-        <v>59.928672</v>
+        <v>55.790529</v>
       </c>
       <c r="B100" t="n">
-        <v>30.420225</v>
+        <v>37.539949</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="n">
-        <v>59.928672</v>
+        <v>55.760251</v>
       </c>
       <c r="B101" t="n">
-        <v>30.420225</v>
+        <v>37.552534</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="n">
-        <v>59.941817</v>
+        <v>55.793085</v>
       </c>
       <c r="B102" t="n">
-        <v>30.2602</v>
+        <v>37.694064</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="n">
-        <v>59.932135</v>
+        <v>55.841898</v>
       </c>
       <c r="B103" t="n">
-        <v>30.470567</v>
+        <v>37.57969</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="n">
-        <v>60.008477</v>
+        <v>55.775935</v>
       </c>
       <c r="B104" t="n">
-        <v>30.294973</v>
+        <v>37.669818</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="n">
-        <v>59.940772</v>
+        <v>55.6766</v>
       </c>
       <c r="B105" t="n">
-        <v>30.290113</v>
+        <v>37.671633</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="n">
-        <v>59.980745</v>
+        <v>55.755819</v>
       </c>
       <c r="B106" t="n">
-        <v>30.388506</v>
+        <v>37.617644</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="n">
-        <v>59.720608</v>
+        <v>60.380048</v>
       </c>
       <c r="B107" t="n">
-        <v>30.429244</v>
+        <v>30.202052</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="n">
-        <v>59.997923</v>
+        <v>55.755819</v>
       </c>
       <c r="B108" t="n">
-        <v>30.260738</v>
+        <v>37.617644</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="n">
-        <v>59.870696</v>
+        <v>55.892567</v>
       </c>
       <c r="B109" t="n">
-        <v>30.448522</v>
+        <v>37.667995</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="n">
-        <v>59.987326</v>
+        <v>55.886494</v>
       </c>
       <c r="B110" t="n">
-        <v>30.292781</v>
+        <v>37.359361</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="n">
-        <v>59.947545</v>
+        <v>55.831555</v>
       </c>
       <c r="B111" t="n">
-        <v>30.361359</v>
+        <v>37.591162</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="n">
-        <v>59.915413</v>
+        <v>55.705863</v>
       </c>
       <c r="B112" t="n">
-        <v>30.310343</v>
+        <v>37.82785</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="n">
-        <v>59.907212</v>
+        <v>55.755115</v>
       </c>
       <c r="B113" t="n">
-        <v>30.299465</v>
+        <v>37.626241</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="n">
-        <v>59.916189</v>
+        <v>55.839062</v>
       </c>
       <c r="B114" t="n">
-        <v>30.339296</v>
+        <v>37.528109</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="n">
-        <v>59.924366</v>
+        <v>55.712092</v>
       </c>
       <c r="B115" t="n">
-        <v>30.296348</v>
+        <v>37.744118</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="n">
-        <v>59.91683</v>
+        <v>55.573037</v>
       </c>
       <c r="B116" t="n">
-        <v>29.642042</v>
+        <v>37.755958</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="n">
-        <v>59.924366</v>
+        <v>55.71414</v>
       </c>
       <c r="B117" t="n">
-        <v>30.296348</v>
+        <v>37.794433</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="n">
-        <v>59.914191</v>
+        <v>55.727095</v>
       </c>
       <c r="B118" t="n">
-        <v>30.337176</v>
+        <v>37.651726</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="n">
-        <v>59.900421</v>
+        <v>55.793045</v>
       </c>
       <c r="B119" t="n">
-        <v>30.268186</v>
+        <v>37.708751</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="n">
-        <v>59.92405</v>
+        <v>55.681585</v>
       </c>
       <c r="B120" t="n">
-        <v>30.292602</v>
+        <v>37.746418</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="n">
-        <v>59.853731</v>
+        <v>55.8375</v>
       </c>
       <c r="B121" t="n">
-        <v>30.039079</v>
+        <v>37.46114</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="n">
-        <v>59.909617</v>
+        <v>55.777049</v>
       </c>
       <c r="B122" t="n">
-        <v>30.27477</v>
+        <v>37.688306</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="n">
-        <v>59.997352</v>
+        <v>55.757642</v>
       </c>
       <c r="B123" t="n">
-        <v>30.362419</v>
+        <v>37.635045</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="n">
-        <v>59.836201</v>
+        <v>55.788515</v>
       </c>
       <c r="B124" t="n">
-        <v>30.215275</v>
+        <v>37.613889</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="n">
-        <v>59.939099</v>
+        <v>55.757404</v>
       </c>
       <c r="B125" t="n">
-        <v>30.315877</v>
+        <v>37.53437</v>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="n">
-        <v>59.972348</v>
+        <v>55.821163</v>
       </c>
       <c r="B126" t="n">
-        <v>30.38591</v>
+        <v>37.796921</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="n">
-        <v>59.941502</v>
+        <v>55.745605</v>
       </c>
       <c r="B127" t="n">
-        <v>30.393501</v>
+        <v>37.796229</v>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="n">
-        <v>59.858539</v>
+        <v>55.792463</v>
       </c>
       <c r="B128" t="n">
-        <v>30.327681</v>
+        <v>37.790408</v>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="n">
-        <v>60.042999</v>
+        <v>55.790489</v>
       </c>
       <c r="B129" t="n">
-        <v>30.392081</v>
+        <v>37.747056</v>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="n">
-        <v>59.930273</v>
+        <v>55.773191</v>
       </c>
       <c r="B130" t="n">
-        <v>30.370207</v>
+        <v>37.526968</v>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="n">
-        <v>59.934997</v>
+        <v>55.752886</v>
       </c>
       <c r="B131" t="n">
-        <v>30.380304</v>
+        <v>37.582089</v>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="n">
-        <v>59.92235</v>
+        <v>55.72709</v>
       </c>
       <c r="B132" t="n">
-        <v>30.327897</v>
+        <v>37.610943</v>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="n">
-        <v>59.747806</v>
+        <v>55.82041</v>
       </c>
       <c r="B133" t="n">
-        <v>30.605233</v>
+        <v>37.758644</v>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="n">
-        <v>59.871924</v>
+        <v>55.659358</v>
       </c>
       <c r="B134" t="n">
-        <v>29.913576</v>
+        <v>37.757449</v>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="n">
-        <v>59.943372</v>
+        <v>55.800651</v>
       </c>
       <c r="B135" t="n">
-        <v>30.281238</v>
+        <v>37.495464</v>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="n">
-        <v>59.995476</v>
+        <v>55.734304</v>
       </c>
       <c r="B136" t="n">
-        <v>30.202348</v>
+        <v>37.705823</v>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="n">
-        <v>59.867552</v>
+        <v>55.621673</v>
       </c>
       <c r="B137" t="n">
-        <v>30.460632</v>
+        <v>37.743103</v>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="n">
-        <v>59.919364</v>
+        <v>55.816925</v>
       </c>
       <c r="B138" t="n">
-        <v>30.440698</v>
+        <v>37.78288</v>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="n">
-        <v>59.918354</v>
+        <v>55.665599</v>
       </c>
       <c r="B139" t="n">
-        <v>30.349824</v>
+        <v>37.650738</v>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="n">
-        <v>59.811093</v>
+        <v>55.707116</v>
       </c>
       <c r="B140" t="n">
-        <v>30.569714</v>
+        <v>37.019833</v>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="n">
-        <v>59.837074</v>
+        <v>55.758114</v>
       </c>
       <c r="B141" t="n">
-        <v>30.141927</v>
+        <v>37.839007</v>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="n">
-        <v>59.924582</v>
+        <v>55.885327</v>
       </c>
       <c r="B142" t="n">
-        <v>30.323342</v>
+        <v>37.60611</v>
       </c>
     </row>
     <row r="143">
       <c r="A143" t="n">
-        <v>59.924645</v>
+        <v>55.787973</v>
       </c>
       <c r="B143" t="n">
-        <v>30.303382</v>
+        <v>37.511266</v>
       </c>
     </row>
     <row r="144">
       <c r="A144" t="n">
-        <v>59.902686</v>
+        <v>55.684945</v>
       </c>
       <c r="B144" t="n">
-        <v>30.337275</v>
+        <v>37.85382</v>
       </c>
     </row>
     <row r="145">
       <c r="A145" t="n">
-        <v>59.925525</v>
+        <v>55.752095</v>
       </c>
       <c r="B145" t="n">
-        <v>30.349294</v>
+        <v>37.761815</v>
       </c>
     </row>
     <row r="146">
       <c r="A146" t="n">
-        <v>60.092137</v>
+        <v>55.60967</v>
       </c>
       <c r="B146" t="n">
-        <v>29.966774</v>
+        <v>37.73076</v>
       </c>
     </row>
     <row r="147">
       <c r="A147" t="n">
-        <v>59.940627</v>
+        <v>55.624332</v>
       </c>
       <c r="B147" t="n">
-        <v>30.348827</v>
+        <v>37.743992</v>
       </c>
     </row>
     <row r="148">
       <c r="A148" t="n">
-        <v>59.732838</v>
+        <v>55.766207</v>
       </c>
       <c r="B148" t="n">
-        <v>30.083636</v>
+        <v>37.732467</v>
       </c>
     </row>
     <row r="149">
       <c r="A149" t="n">
-        <v>59.983374</v>
+        <v>55.711681</v>
       </c>
       <c r="B149" t="n">
-        <v>30.34704</v>
+        <v>37.730733</v>
       </c>
     </row>
     <row r="150">
       <c r="A150" t="n">
-        <v>59.928708</v>
+        <v>55.726325</v>
       </c>
       <c r="B150" t="n">
-        <v>30.242754</v>
+        <v>37.680931</v>
       </c>
     </row>
     <row r="151">
       <c r="A151" t="n">
-        <v>59.841794</v>
+        <v>55.739392</v>
       </c>
       <c r="B151" t="n">
-        <v>30.424187</v>
+        <v>37.493731</v>
       </c>
     </row>
     <row r="152">
       <c r="A152" t="n">
-        <v>60.013204</v>
+        <v>55.890997</v>
       </c>
       <c r="B152" t="n">
-        <v>30.320503</v>
+        <v>37.617096</v>
       </c>
     </row>
     <row r="153">
       <c r="A153" t="n">
-        <v>59.785975</v>
+        <v>55.779656</v>
       </c>
       <c r="B153" t="n">
-        <v>30.623388</v>
+        <v>37.603837</v>
       </c>
     </row>
     <row r="154">
       <c r="A154" t="n">
-        <v>59.917804</v>
+        <v>55.784131</v>
       </c>
       <c r="B154" t="n">
-        <v>30.278202</v>
+        <v>37.428288</v>
       </c>
     </row>
     <row r="155">
       <c r="A155" t="n">
-        <v>59.907316</v>
+        <v>55.839062</v>
       </c>
       <c r="B155" t="n">
-        <v>30.295575</v>
+        <v>37.528109</v>
       </c>
     </row>
     <row r="156">
       <c r="A156" t="n">
-        <v>59.918566</v>
+        <v>55.825664</v>
       </c>
       <c r="B156" t="n">
-        <v>30.299043</v>
+        <v>37.966514</v>
       </c>
     </row>
     <row r="157">
       <c r="A157" t="n">
-        <v>59.802372</v>
+        <v>55.649261</v>
       </c>
       <c r="B157" t="n">
-        <v>30.513515</v>
+        <v>37.594638</v>
       </c>
     </row>
     <row r="158">
       <c r="A158" t="n">
-        <v>60.20313</v>
+        <v>55.828925</v>
       </c>
       <c r="B158" t="n">
-        <v>29.69418</v>
+        <v>37.701322</v>
       </c>
     </row>
     <row r="159">
       <c r="A159" t="n">
-        <v>59.886293</v>
+        <v>55.826347</v>
       </c>
       <c r="B159" t="n">
-        <v>30.479092</v>
+        <v>37.571022</v>
       </c>
     </row>
     <row r="160">
       <c r="A160" t="n">
-        <v>59.859926</v>
+        <v>55.891809</v>
       </c>
       <c r="B160" t="n">
-        <v>29.992816</v>
+        <v>37.748735</v>
       </c>
     </row>
     <row r="161">
       <c r="A161" t="n">
-        <v>59.860328</v>
+        <v>55.841898</v>
       </c>
       <c r="B161" t="n">
-        <v>30.328238</v>
+        <v>37.57969</v>
       </c>
     </row>
     <row r="162">
       <c r="A162" t="n">
-        <v>60.019019</v>
+        <v>55.798141</v>
       </c>
       <c r="B162" t="n">
-        <v>30.283475</v>
+        <v>37.518093</v>
       </c>
     </row>
     <row r="163">
       <c r="A163" t="n">
-        <v>59.900809</v>
+        <v>55.620209</v>
       </c>
       <c r="B163" t="n">
-        <v>29.712488</v>
+        <v>37.588925</v>
       </c>
     </row>
     <row r="164">
       <c r="A164" t="n">
-        <v>59.95229</v>
+        <v>55.838374</v>
       </c>
       <c r="B164" t="n">
-        <v>30.213846</v>
+        <v>37.42615</v>
       </c>
     </row>
     <row r="165">
       <c r="A165" t="n">
-        <v>59.84145</v>
+        <v>55.755864</v>
       </c>
       <c r="B165" t="n">
-        <v>29.898789</v>
+        <v>37.617698</v>
       </c>
     </row>
     <row r="166">
       <c r="A166" t="n">
-        <v>59.933059</v>
+        <v>55.809282</v>
       </c>
       <c r="B166" t="n">
-        <v>30.27486</v>
+        <v>37.793921</v>
       </c>
     </row>
     <row r="167">
       <c r="A167" t="n">
-        <v>59.954043</v>
+        <v>55.747323</v>
       </c>
       <c r="B167" t="n">
-        <v>30.217745</v>
+        <v>37.396371</v>
       </c>
     </row>
     <row r="168">
       <c r="A168" t="n">
-        <v>59.954773</v>
+        <v>55.866627</v>
       </c>
       <c r="B168" t="n">
-        <v>30.214745</v>
+        <v>37.445491</v>
       </c>
     </row>
     <row r="169">
       <c r="A169" t="n">
-        <v>59.943543</v>
+        <v>55.921758</v>
       </c>
       <c r="B169" t="n">
-        <v>30.27088</v>
+        <v>37.719441</v>
       </c>
     </row>
     <row r="170">
       <c r="A170" t="n">
-        <v>59.945639</v>
+        <v>55.836777</v>
       </c>
       <c r="B170" t="n">
-        <v>30.216434</v>
+        <v>37.354644</v>
       </c>
     </row>
     <row r="171">
       <c r="A171" t="n">
-        <v>59.945639</v>
+        <v>55.745878</v>
       </c>
       <c r="B171" t="n">
-        <v>30.267916</v>
+        <v>37.837731</v>
       </c>
     </row>
     <row r="172">
       <c r="A172" t="n">
-        <v>59.936169</v>
+        <v>55.862161</v>
       </c>
       <c r="B172" t="n">
-        <v>30.236044</v>
+        <v>37.612964</v>
       </c>
     </row>
     <row r="173">
       <c r="A173" t="n">
-        <v>59.947338</v>
+        <v>55.762216</v>
       </c>
       <c r="B173" t="n">
-        <v>30.260577</v>
+        <v>37.538296</v>
       </c>
     </row>
     <row r="174">
       <c r="A174" t="n">
-        <v>60.050475</v>
+        <v>55.733913</v>
       </c>
       <c r="B174" t="n">
-        <v>30.311143</v>
+        <v>37.56459</v>
       </c>
     </row>
     <row r="175">
       <c r="A175" t="n">
-        <v>60.043952</v>
+        <v>55.799487</v>
       </c>
       <c r="B175" t="n">
-        <v>30.324079</v>
+        <v>37.794576</v>
       </c>
     </row>
     <row r="176">
       <c r="A176" t="n">
-        <v>59.911701</v>
+        <v>55.76562</v>
       </c>
       <c r="B176" t="n">
-        <v>30.279091</v>
+        <v>37.726493</v>
       </c>
     </row>
     <row r="177">
       <c r="A177" t="n">
-        <v>59.973987</v>
+        <v>55.755864</v>
       </c>
       <c r="B177" t="n">
-        <v>30.306445</v>
+        <v>37.617698</v>
       </c>
     </row>
     <row r="178">
       <c r="A178" t="n">
-        <v>60.048494</v>
+        <v>55.652684</v>
       </c>
       <c r="B178" t="n">
-        <v>30.367261</v>
+        <v>37.76769</v>
       </c>
     </row>
     <row r="179">
       <c r="A179" t="n">
-        <v>60.052816</v>
+        <v>55.741439</v>
       </c>
       <c r="B179" t="n">
-        <v>30.355098</v>
+        <v>37.657628</v>
       </c>
     </row>
     <row r="180">
       <c r="A180" t="n">
-        <v>60.047236</v>
+        <v>55.677169</v>
       </c>
       <c r="B180" t="n">
-        <v>30.451109</v>
+        <v>37.656164</v>
       </c>
     </row>
     <row r="181">
       <c r="A181" t="n">
-        <v>60.030146</v>
+        <v>55.884701</v>
       </c>
       <c r="B181" t="n">
-        <v>30.309248</v>
+        <v>37.737417</v>
       </c>
     </row>
     <row r="182">
       <c r="A182" t="n">
-        <v>59.981321</v>
+        <v>55.678605</v>
       </c>
       <c r="B182" t="n">
-        <v>30.353813</v>
+        <v>37.759147</v>
       </c>
     </row>
     <row r="183">
       <c r="A183" t="n">
-        <v>60.037063</v>
+        <v>55.608923</v>
       </c>
       <c r="B183" t="n">
-        <v>30.33149</v>
+        <v>37.71053</v>
       </c>
     </row>
     <row r="184">
       <c r="A184" t="n">
-        <v>60.088987</v>
+        <v>55.882889</v>
       </c>
       <c r="B184" t="n">
-        <v>30.275031</v>
+        <v>37.660449</v>
       </c>
     </row>
     <row r="185">
       <c r="A185" t="n">
-        <v>60.075488</v>
+        <v>55.75824</v>
       </c>
       <c r="B185" t="n">
-        <v>30.293249</v>
+        <v>37.8419</v>
       </c>
     </row>
     <row r="186">
       <c r="A186" t="n">
-        <v>60.034843</v>
+        <v>55.808902</v>
       </c>
       <c r="B186" t="n">
-        <v>30.393518</v>
+        <v>37.76999</v>
       </c>
     </row>
     <row r="187">
       <c r="A187" t="n">
-        <v>60.000353</v>
+        <v>55.860726</v>
       </c>
       <c r="B187" t="n">
-        <v>30.435093</v>
+        <v>37.502902</v>
       </c>
     </row>
     <row r="188">
       <c r="A188" t="n">
-        <v>59.997793</v>
+        <v>55.746405</v>
       </c>
       <c r="B188" t="n">
-        <v>30.448909</v>
+        <v>37.592689</v>
       </c>
     </row>
     <row r="189">
       <c r="A189" t="n">
-        <v>60.013312</v>
+        <v>55.755864</v>
       </c>
       <c r="B189" t="n">
-        <v>30.36055</v>
+        <v>37.617698</v>
       </c>
     </row>
     <row r="190">
       <c r="A190" t="n">
-        <v>59.974671</v>
+        <v>55.701907</v>
       </c>
       <c r="B190" t="n">
-        <v>30.387688</v>
+        <v>37.788585</v>
       </c>
     </row>
     <row r="191">
       <c r="A191" t="n">
-        <v>60.128144</v>
+        <v>55.758681</v>
       </c>
       <c r="B191" t="n">
-        <v>30.439701</v>
+        <v>37.642069</v>
       </c>
     </row>
     <row r="192">
       <c r="A192" t="n">
-        <v>59.97893</v>
+        <v>55.875107</v>
       </c>
       <c r="B192" t="n">
-        <v>30.353472</v>
+        <v>37.70912</v>
       </c>
     </row>
     <row r="193">
       <c r="A193" t="n">
-        <v>60.020071</v>
+        <v>55.774836</v>
       </c>
       <c r="B193" t="n">
-        <v>30.411494</v>
+        <v>37.632664</v>
       </c>
     </row>
     <row r="194">
       <c r="A194" t="n">
-        <v>60.00895</v>
+        <v>55.684945</v>
       </c>
       <c r="B194" t="n">
-        <v>30.344255</v>
+        <v>37.85382</v>
       </c>
     </row>
     <row r="195">
       <c r="A195" t="n">
-        <v>59.89292</v>
+        <v>55.780674</v>
       </c>
       <c r="B195" t="n">
-        <v>30.266542</v>
+        <v>37.619495</v>
       </c>
     </row>
     <row r="196">
       <c r="A196" t="n">
-        <v>59.876865</v>
+        <v>55.716159</v>
       </c>
       <c r="B196" t="n">
-        <v>30.263999</v>
+        <v>37.566332</v>
       </c>
     </row>
     <row r="197">
       <c r="A197" t="n">
-        <v>59.868401</v>
+        <v>55.755864</v>
       </c>
       <c r="B197" t="n">
-        <v>30.248764</v>
+        <v>37.617698</v>
       </c>
     </row>
     <row r="198">
       <c r="A198" t="n">
-        <v>59.778679</v>
+        <v>55.762981</v>
       </c>
       <c r="B198" t="n">
-        <v>30.130743</v>
+        <v>37.646193</v>
       </c>
     </row>
     <row r="199">
       <c r="A199" t="n">
-        <v>59.868699</v>
+        <v>55.76761</v>
       </c>
       <c r="B199" t="n">
-        <v>30.238631</v>
+        <v>37.927249</v>
       </c>
     </row>
     <row r="200">
       <c r="A200" t="n">
-        <v>59.882939</v>
+        <v>55.674504</v>
       </c>
       <c r="B200" t="n">
-        <v>30.267916</v>
+        <v>37.504564</v>
       </c>
     </row>
     <row r="201">
       <c r="A201" t="n">
-        <v>59.867145</v>
+        <v>55.680549</v>
       </c>
       <c r="B201" t="n">
-        <v>30.259454</v>
+        <v>37.864959</v>
       </c>
     </row>
     <row r="202">
       <c r="A202" t="n">
-        <v>59.846554</v>
+        <v>55.683595</v>
       </c>
       <c r="B202" t="n">
-        <v>30.244362</v>
+        <v>37.707143</v>
       </c>
     </row>
     <row r="203">
       <c r="A203" t="n">
-        <v>59.905317</v>
+        <v>55.70246</v>
       </c>
       <c r="B203" t="n">
-        <v>30.270638</v>
+        <v>37.742672</v>
       </c>
     </row>
     <row r="204">
       <c r="A204" t="n">
-        <v>59.935967</v>
+        <v>55.8113</v>
       </c>
       <c r="B204" t="n">
-        <v>30.406589</v>
+        <v>37.62669</v>
       </c>
     </row>
     <row r="205">
       <c r="A205" t="n">
-        <v>59.963052</v>
+        <v>55.719632</v>
       </c>
       <c r="B205" t="n">
-        <v>30.416749</v>
+        <v>37.387729</v>
       </c>
     </row>
     <row r="206">
       <c r="A206" t="n">
-        <v>60.047236</v>
+        <v>55.883429</v>
       </c>
       <c r="B206" t="n">
-        <v>30.451109</v>
+        <v>37.55849</v>
       </c>
     </row>
     <row r="207">
       <c r="A207" t="n">
-        <v>59.958336</v>
+        <v>55.87343</v>
       </c>
       <c r="B207" t="n">
-        <v>30.410434</v>
+        <v>37.520527</v>
       </c>
     </row>
     <row r="208">
       <c r="A208" t="n">
-        <v>59.92309</v>
+        <v>55.688964</v>
       </c>
       <c r="B208" t="n">
-        <v>30.408655</v>
+        <v>37.294385</v>
       </c>
     </row>
     <row r="209">
       <c r="A209" t="n">
-        <v>59.984436</v>
+        <v>55.642393</v>
       </c>
       <c r="B209" t="n">
-        <v>30.507667</v>
+        <v>37.677472</v>
       </c>
     </row>
     <row r="210">
       <c r="A210" t="n">
-        <v>59.973208</v>
+        <v>55.734385</v>
       </c>
       <c r="B210" t="n">
-        <v>30.416956</v>
+        <v>37.655832</v>
       </c>
     </row>
     <row r="211">
       <c r="A211" t="n">
-        <v>59.954858</v>
+        <v>55.859544</v>
       </c>
       <c r="B211" t="n">
-        <v>30.441677</v>
+        <v>37.55743</v>
       </c>
     </row>
     <row r="212">
       <c r="A212" t="n">
-        <v>59.938635</v>
+        <v>55.902813</v>
       </c>
       <c r="B212" t="n">
-        <v>30.487608</v>
+        <v>37.746615</v>
       </c>
     </row>
     <row r="213">
       <c r="A213" t="n">
-        <v>59.961674</v>
+        <v>55.740634</v>
       </c>
       <c r="B213" t="n">
-        <v>30.455664</v>
+        <v>37.435134</v>
       </c>
     </row>
     <row r="214">
       <c r="A214" t="n">
-        <v>59.921962</v>
+        <v>55.711463</v>
       </c>
       <c r="B214" t="n">
-        <v>30.416875</v>
+        <v>37.416808</v>
       </c>
     </row>
     <row r="215">
       <c r="A215" t="n">
-        <v>59.952254</v>
+        <v>55.684686</v>
       </c>
       <c r="B215" t="n">
-        <v>30.408395</v>
+        <v>37.85294</v>
       </c>
     </row>
     <row r="216">
       <c r="A216" t="n">
-        <v>59.95457</v>
+        <v>55.798556</v>
       </c>
       <c r="B216" t="n">
-        <v>30.436215</v>
+        <v>37.582808</v>
       </c>
     </row>
     <row r="217">
       <c r="A217" t="n">
-        <v>59.940114</v>
+        <v>55.780598</v>
       </c>
       <c r="B217" t="n">
-        <v>30.481104</v>
+        <v>37.697019</v>
       </c>
     </row>
     <row r="218">
       <c r="A218" t="n">
-        <v>59.955597</v>
+        <v>55.847113</v>
       </c>
       <c r="B218" t="n">
-        <v>30.491489</v>
+        <v>37.558571</v>
       </c>
     </row>
     <row r="219">
       <c r="A219" t="n">
-        <v>59.828903</v>
+        <v>55.741526</v>
       </c>
       <c r="B219" t="n">
-        <v>30.094604</v>
+        <v>37.67201</v>
       </c>
     </row>
     <row r="220">
       <c r="A220" t="n">
-        <v>59.851096</v>
+        <v>55.602383</v>
       </c>
       <c r="B220" t="n">
-        <v>30.060962</v>
+        <v>37.581406</v>
       </c>
     </row>
     <row r="221">
       <c r="A221" t="n">
-        <v>59.868248</v>
+        <v>55.837616</v>
       </c>
       <c r="B221" t="n">
-        <v>29.977958</v>
+        <v>37.255911</v>
       </c>
     </row>
     <row r="222">
       <c r="A222" t="n">
-        <v>59.709853</v>
+        <v>55.85959</v>
       </c>
       <c r="B222" t="n">
-        <v>30.340365</v>
+        <v>37.640704</v>
       </c>
     </row>
     <row r="223">
       <c r="A223" t="n">
-        <v>59.818807</v>
+        <v>55.873784</v>
       </c>
       <c r="B223" t="n">
-        <v>30.191209</v>
+        <v>37.521623</v>
       </c>
     </row>
     <row r="224">
       <c r="A224" t="n">
-        <v>59.866364</v>
+        <v>55.695053</v>
       </c>
       <c r="B224" t="n">
-        <v>30.355906</v>
+        <v>37.801889</v>
       </c>
     </row>
     <row r="225">
       <c r="A225" t="n">
-        <v>59.885426</v>
+        <v>55.804066</v>
       </c>
       <c r="B225" t="n">
-        <v>30.320072</v>
+        <v>37.398087</v>
       </c>
     </row>
     <row r="226">
       <c r="A226" t="n">
-        <v>59.873419</v>
+        <v>55.933302</v>
       </c>
       <c r="B226" t="n">
-        <v>30.308044</v>
+        <v>37.51423</v>
       </c>
     </row>
     <row r="227">
       <c r="A227" t="n">
-        <v>59.85139</v>
+        <v>55.755864</v>
       </c>
       <c r="B227" t="n">
-        <v>30.339754</v>
+        <v>37.617698</v>
       </c>
     </row>
     <row r="228">
       <c r="A228" t="n">
-        <v>59.889372</v>
+        <v>55.834866</v>
       </c>
       <c r="B228" t="n">
-        <v>30.323333</v>
+        <v>37.447054</v>
       </c>
     </row>
     <row r="229">
       <c r="A229" t="n">
-        <v>59.873329</v>
+        <v>55.804228</v>
       </c>
       <c r="B229" t="n">
-        <v>30.291155</v>
+        <v>37.495994</v>
       </c>
     </row>
     <row r="230">
       <c r="A230" t="n">
-        <v>59.899338</v>
+        <v>55.714937</v>
       </c>
       <c r="B230" t="n">
-        <v>30.340248</v>
+        <v>37.100412</v>
       </c>
     </row>
     <row r="231">
       <c r="A231" t="n">
-        <v>59.897691</v>
+        <v>55.890906</v>
       </c>
       <c r="B231" t="n">
-        <v>30.338398</v>
+        <v>37.624525</v>
       </c>
     </row>
     <row r="232">
       <c r="A232" t="n">
-        <v>59.858801</v>
+        <v>55.755864</v>
       </c>
       <c r="B232" t="n">
-        <v>30.327906</v>
+        <v>37.617698</v>
       </c>
     </row>
     <row r="233">
       <c r="A233" t="n">
-        <v>59.885426</v>
+        <v>55.768724</v>
       </c>
       <c r="B233" t="n">
-        <v>30.320072</v>
+        <v>37.712399</v>
       </c>
     </row>
     <row r="234">
       <c r="A234" t="n">
-        <v>59.888862</v>
+        <v>55.772689</v>
       </c>
       <c r="B234" t="n">
-        <v>30.315823</v>
+        <v>37.687659</v>
       </c>
     </row>
     <row r="235">
       <c r="A235" t="n">
-        <v>59.856786</v>
+        <v>55.669554</v>
       </c>
       <c r="B235" t="n">
-        <v>30.361305</v>
+        <v>37.742663</v>
       </c>
     </row>
     <row r="236">
       <c r="A236" t="n">
-        <v>59.858363</v>
+        <v>55.868304</v>
       </c>
       <c r="B236" t="n">
-        <v>30.319875</v>
+        <v>37.498213</v>
       </c>
     </row>
     <row r="237">
       <c r="A237" t="n">
-        <v>59.843091</v>
+        <v>55.863752</v>
       </c>
       <c r="B237" t="n">
-        <v>30.321977</v>
+        <v>37.594108</v>
       </c>
     </row>
     <row r="238">
       <c r="A238" t="n">
-        <v>59.888212</v>
+        <v>55.591177</v>
       </c>
       <c r="B238" t="n">
-        <v>30.331948</v>
+        <v>37.761222</v>
       </c>
     </row>
     <row r="239">
       <c r="A239" t="n">
-        <v>59.840709</v>
+        <v>55.613773</v>
       </c>
       <c r="B239" t="n">
-        <v>30.339826</v>
+        <v>37.538799</v>
       </c>
     </row>
     <row r="240">
       <c r="A240" t="n">
-        <v>59.860328</v>
+        <v>55.755864</v>
       </c>
       <c r="B240" t="n">
-        <v>30.328238</v>
+        <v>37.617698</v>
       </c>
     </row>
     <row r="241">
       <c r="A241" t="n">
-        <v>59.892852</v>
+        <v>55.759821</v>
       </c>
       <c r="B241" t="n">
-        <v>30.436575</v>
+        <v>37.575396</v>
       </c>
     </row>
     <row r="242">
       <c r="A242" t="n">
-        <v>59.899058</v>
+        <v>55.851924</v>
       </c>
       <c r="B242" t="n">
-        <v>30.427933</v>
+        <v>37.604628</v>
       </c>
     </row>
     <row r="243">
       <c r="A243" t="n">
-        <v>59.884243</v>
+        <v>55.838379</v>
       </c>
       <c r="B243" t="n">
-        <v>30.438416</v>
+        <v>37.54771</v>
       </c>
     </row>
     <row r="244">
       <c r="A244" t="n">
-        <v>59.944711</v>
+        <v>55.779565</v>
       </c>
       <c r="B244" t="n">
-        <v>30.494462</v>
+        <v>37.601421</v>
       </c>
     </row>
     <row r="245">
       <c r="A245" t="n">
-        <v>59.906639</v>
+        <v>55.755864</v>
       </c>
       <c r="B245" t="n">
-        <v>30.404667</v>
+        <v>37.617698</v>
       </c>
     </row>
     <row r="246">
       <c r="A246" t="n">
-        <v>59.945639</v>
+        <v>55.851576</v>
       </c>
       <c r="B246" t="n">
-        <v>30.267916</v>
+        <v>37.53199</v>
       </c>
     </row>
     <row r="247">
       <c r="A247" t="n">
-        <v>59.922269</v>
+        <v>55.791891</v>
       </c>
       <c r="B247" t="n">
-        <v>30.444183</v>
+        <v>37.670744</v>
       </c>
     </row>
     <row r="248">
       <c r="A248" t="n">
-        <v>59.861196</v>
+        <v>55.755181</v>
       </c>
       <c r="B248" t="n">
-        <v>30.476065</v>
+        <v>37.66927</v>
       </c>
     </row>
     <row r="249">
       <c r="A249" t="n">
-        <v>59.943214</v>
+        <v>55.896337</v>
       </c>
       <c r="B249" t="n">
-        <v>30.479442</v>
+        <v>37.609146</v>
       </c>
     </row>
     <row r="250">
       <c r="A250" t="n">
-        <v>59.865</v>
+        <v>55.743953</v>
       </c>
       <c r="B250" t="n">
-        <v>30.44598</v>
+        <v>37.846993</v>
       </c>
     </row>
     <row r="251">
       <c r="A251" t="n">
-        <v>59.966349</v>
+        <v>55.680524</v>
       </c>
       <c r="B251" t="n">
-        <v>30.474106</v>
+        <v>37.74931</v>
       </c>
     </row>
     <row r="252">
       <c r="A252" t="n">
-        <v>59.899712</v>
+        <v>55.809874</v>
       </c>
       <c r="B252" t="n">
-        <v>30.423423</v>
+        <v>37.476654</v>
       </c>
     </row>
     <row r="253">
       <c r="A253" t="n">
-        <v>59.865587</v>
+        <v>55.792463</v>
       </c>
       <c r="B253" t="n">
-        <v>30.466013</v>
+        <v>37.790408</v>
       </c>
     </row>
     <row r="254">
       <c r="A254" t="n">
-        <v>59.882171</v>
+        <v>55.766207</v>
       </c>
       <c r="B254" t="n">
-        <v>30.489369</v>
+        <v>37.732467</v>
       </c>
     </row>
     <row r="255">
       <c r="A255" t="n">
-        <v>59.899329</v>
+        <v>55.673692</v>
       </c>
       <c r="B255" t="n">
-        <v>30.493609</v>
+        <v>37.738243</v>
       </c>
     </row>
     <row r="256">
       <c r="A256" t="n">
-        <v>59.968232</v>
+        <v>55.729153</v>
       </c>
       <c r="B256" t="n">
-        <v>30.308843</v>
+        <v>37.571147</v>
       </c>
     </row>
     <row r="257">
       <c r="A257" t="n">
-        <v>59.962836</v>
+        <v>55.729153</v>
       </c>
       <c r="B257" t="n">
-        <v>30.30136</v>
+        <v>37.571147</v>
       </c>
     </row>
     <row r="258">
       <c r="A258" t="n">
-        <v>59.958246</v>
+        <v>55.763265</v>
       </c>
       <c r="B258" t="n">
-        <v>30.263344</v>
+        <v>37.566162</v>
       </c>
     </row>
     <row r="259">
       <c r="A259" t="n">
-        <v>59.968025</v>
+        <v>55.734004</v>
       </c>
       <c r="B259" t="n">
-        <v>30.263281</v>
+        <v>37.659452</v>
       </c>
     </row>
     <row r="260">
       <c r="A260" t="n">
-        <v>59.958683</v>
+        <v>55.658733</v>
       </c>
       <c r="B260" t="n">
-        <v>30.304765</v>
+        <v>37.736563</v>
       </c>
     </row>
     <row r="261">
       <c r="A261" t="n">
-        <v>60.026963</v>
+        <v>55.681742</v>
       </c>
       <c r="B261" t="n">
-        <v>30.298638</v>
+        <v>37.92865</v>
       </c>
     </row>
     <row r="262">
       <c r="A262" t="n">
-        <v>59.991894</v>
+        <v>55.801546</v>
       </c>
       <c r="B262" t="n">
-        <v>30.321177</v>
+        <v>37.576241</v>
       </c>
     </row>
     <row r="263">
       <c r="A263" t="n">
-        <v>59.995476</v>
+        <v>55.735713</v>
       </c>
       <c r="B263" t="n">
-        <v>30.202348</v>
+        <v>37.689932</v>
       </c>
     </row>
     <row r="264">
       <c r="A264" t="n">
-        <v>59.995476</v>
+        <v>55.622324</v>
       </c>
       <c r="B264" t="n">
-        <v>30.202348</v>
+        <v>37.667662</v>
       </c>
     </row>
     <row r="265">
       <c r="A265" t="n">
-        <v>60.017976</v>
+        <v>55.742777</v>
       </c>
       <c r="B265" t="n">
-        <v>30.277699</v>
+        <v>37.609667</v>
       </c>
     </row>
     <row r="266">
       <c r="A266" t="n">
-        <v>59.998256</v>
+        <v>55.798672</v>
       </c>
       <c r="B266" t="n">
-        <v>30.293096</v>
+        <v>37.718983</v>
       </c>
     </row>
     <row r="267">
       <c r="A267" t="n">
-        <v>59.938955</v>
+        <v>55.83893</v>
       </c>
       <c r="B267" t="n">
-        <v>30.315644</v>
+        <v>37.652777</v>
       </c>
     </row>
     <row r="268">
       <c r="A268" t="n">
-        <v>60.017535</v>
+        <v>55.87693</v>
       </c>
       <c r="B268" t="n">
-        <v>30.283035</v>
+        <v>37.712722</v>
       </c>
     </row>
     <row r="269">
       <c r="A269" t="n">
-        <v>59.942403</v>
+        <v>55.809272</v>
       </c>
       <c r="B269" t="n">
-        <v>30.352052</v>
+        <v>37.725191</v>
       </c>
     </row>
     <row r="270">
       <c r="A270" t="n">
-        <v>60.033616</v>
+        <v>55.642738</v>
       </c>
       <c r="B270" t="n">
-        <v>30.244407</v>
+        <v>37.793624</v>
       </c>
     </row>
     <row r="271">
       <c r="A271" t="n">
-        <v>59.995017</v>
+        <v>55.786814</v>
       </c>
       <c r="B271" t="n">
-        <v>30.148781</v>
+        <v>37.631146</v>
       </c>
     </row>
     <row r="272">
       <c r="A272" t="n">
-        <v>59.910496</v>
+        <v>55.758792</v>
       </c>
       <c r="B272" t="n">
-        <v>30.254298</v>
+        <v>37.704071</v>
       </c>
     </row>
     <row r="273">
       <c r="A273" t="n">
-        <v>59.997982</v>
+        <v>55.816166</v>
       </c>
       <c r="B273" t="n">
-        <v>30.271617</v>
+        <v>37.86469</v>
       </c>
     </row>
     <row r="274">
       <c r="A274" t="n">
-        <v>59.983504</v>
+        <v>55.748052</v>
       </c>
       <c r="B274" t="n">
-        <v>30.219605</v>
+        <v>38.034651</v>
       </c>
     </row>
     <row r="275">
       <c r="A275" t="n">
-        <v>59.864286</v>
+        <v>55.755864</v>
       </c>
       <c r="B275" t="n">
-        <v>30.399088</v>
+        <v>37.617698</v>
       </c>
     </row>
     <row r="276">
       <c r="A276" t="n">
-        <v>59.862976</v>
+        <v>55.755864</v>
       </c>
       <c r="B276" t="n">
-        <v>30.415563</v>
+        <v>37.617698</v>
       </c>
     </row>
     <row r="277">
       <c r="A277" t="n">
-        <v>60.016645</v>
+        <v>55.38686</v>
       </c>
       <c r="B277" t="n">
-        <v>30.292871</v>
+        <v>37.837264</v>
       </c>
     </row>
     <row r="278">
       <c r="A278" t="n">
-        <v>59.841794</v>
+        <v>55.780912</v>
       </c>
       <c r="B278" t="n">
-        <v>30.424187</v>
+        <v>37.607053</v>
       </c>
     </row>
     <row r="279">
       <c r="A279" t="n">
-        <v>59.884085</v>
+        <v>55.676935</v>
       </c>
       <c r="B279" t="n">
-        <v>30.390761</v>
+        <v>37.744953</v>
       </c>
     </row>
     <row r="280">
       <c r="A280" t="n">
-        <v>59.939591</v>
+        <v>55.723577</v>
       </c>
       <c r="B280" t="n">
-        <v>30.361296</v>
+        <v>37.677014</v>
       </c>
     </row>
     <row r="281">
       <c r="A281" t="n">
-        <v>59.850477</v>
+        <v>55.683595</v>
       </c>
       <c r="B281" t="n">
-        <v>30.368698</v>
+        <v>37.707143</v>
       </c>
     </row>
     <row r="282">
       <c r="A282" t="n">
-        <v>59.857111</v>
+        <v>55.809879</v>
       </c>
       <c r="B282" t="n">
-        <v>30.365725</v>
+        <v>37.35336</v>
       </c>
     </row>
     <row r="283">
       <c r="A283" t="n">
-        <v>59.905782</v>
+        <v>55.660404</v>
       </c>
       <c r="B283" t="n">
-        <v>30.364656</v>
+        <v>37.62519</v>
       </c>
     </row>
     <row r="284">
       <c r="A284" t="n">
-        <v>59.839086</v>
+        <v>55.543521</v>
       </c>
       <c r="B284" t="n">
-        <v>30.38494</v>
+        <v>37.511544</v>
       </c>
     </row>
     <row r="285">
       <c r="A285" t="n">
-        <v>59.942025</v>
+        <v>55.72669</v>
       </c>
       <c r="B285" t="n">
-        <v>30.344956</v>
+        <v>37.644917</v>
       </c>
     </row>
     <row r="286">
       <c r="A286" t="n">
-        <v>59.944368</v>
+        <v>55.783904</v>
       </c>
       <c r="B286" t="n">
-        <v>30.345566</v>
+        <v>37.738054</v>
       </c>
     </row>
     <row r="287">
       <c r="A287" t="n">
-        <v>59.939523</v>
+        <v>55.879106</v>
       </c>
       <c r="B287" t="n">
-        <v>30.358484</v>
+        <v>37.712848</v>
       </c>
     </row>
     <row r="288">
       <c r="A288" t="n">
-        <v>59.949195</v>
+        <v>55.756336</v>
       </c>
       <c r="B288" t="n">
-        <v>30.35269</v>
+        <v>37.788279</v>
       </c>
     </row>
     <row r="289">
       <c r="A289" t="n">
-        <v>59.937418</v>
+        <v>55.680311</v>
       </c>
       <c r="B289" t="n">
-        <v>30.378023</v>
+        <v>37.623492</v>
       </c>
     </row>
     <row r="290">
       <c r="A290" t="n">
-        <v>59.926449</v>
+        <v>55.894005</v>
       </c>
       <c r="B290" t="n">
-        <v>30.333134</v>
+        <v>37.729583</v>
       </c>
     </row>
     <row r="291">
       <c r="A291" t="n">
-        <v>59.924938</v>
+        <v>55.764101</v>
       </c>
       <c r="B291" t="n">
-        <v>30.344722</v>
+        <v>37.854395</v>
       </c>
     </row>
     <row r="292">
       <c r="A292" t="n">
-        <v>59.934344</v>
+        <v>55.764268</v>
       </c>
       <c r="B292" t="n">
-        <v>30.392566</v>
+        <v>37.622073</v>
       </c>
     </row>
     <row r="293">
       <c r="A293" t="n">
-        <v>59.941615</v>
+        <v>55.796835</v>
       </c>
       <c r="B293" t="n">
-        <v>30.351693</v>
+        <v>37.455247</v>
       </c>
     </row>
     <row r="294">
       <c r="A294" t="n">
-        <v>59.939613</v>
+        <v>55.884282</v>
       </c>
       <c r="B294" t="n">
-        <v>30.37725</v>
+        <v>37.558841</v>
       </c>
     </row>
     <row r="295">
       <c r="A295" t="n">
-        <v>59.836893</v>
+        <v>55.778396</v>
       </c>
       <c r="B295" t="n">
-        <v>29.90541</v>
+        <v>37.639401</v>
       </c>
     </row>
     <row r="296">
       <c r="A296" t="n">
-        <v>59.927915</v>
+        <v>55.843591</v>
       </c>
       <c r="B296" t="n">
-        <v>30.338425</v>
+        <v>37.423446</v>
       </c>
     </row>
     <row r="297">
       <c r="A297" t="n">
-        <v>59.91724</v>
+        <v>55.873521</v>
       </c>
       <c r="B297" t="n">
-        <v>30.345279</v>
+        <v>37.673169</v>
       </c>
     </row>
     <row r="298">
       <c r="A298" t="n">
-        <v>59.947554</v>
+        <v>55.762961</v>
       </c>
       <c r="B298" t="n">
-        <v>30.360398</v>
+        <v>37.523115</v>
       </c>
     </row>
     <row r="299">
       <c r="A299" t="n">
-        <v>59.92157</v>
+        <v>55.7407</v>
       </c>
       <c r="B299" t="n">
-        <v>30.345611</v>
+        <v>37.670133</v>
       </c>
     </row>
     <row r="300">
       <c r="A300" t="n">
-        <v>59.912098</v>
+        <v>55.771332</v>
       </c>
       <c r="B300" t="n">
-        <v>30.354262</v>
+        <v>37.614815</v>
       </c>
     </row>
     <row r="301">
       <c r="A301" t="n">
-        <v>60.033926</v>
+        <v>55.763614</v>
       </c>
       <c r="B301" t="n">
-        <v>30.313532</v>
+        <v>37.565856</v>
       </c>
     </row>
     <row r="302">
       <c r="A302" t="n">
-        <v>59.842725</v>
+        <v>55.73403</v>
       </c>
       <c r="B302" t="n">
-        <v>30.31841</v>
+        <v>37.66353</v>
       </c>
     </row>
     <row r="303">
       <c r="A303" t="n">
-        <v>60.039099</v>
+        <v>55.837884</v>
       </c>
       <c r="B303" t="n">
-        <v>30.299106</v>
+        <v>37.636437</v>
       </c>
     </row>
     <row r="304">
       <c r="A304" t="n">
-        <v>59.841844</v>
+        <v>55.776502</v>
       </c>
       <c r="B304" t="n">
-        <v>30.349375</v>
+        <v>37.537119</v>
       </c>
     </row>
     <row r="305">
       <c r="A305" t="n">
-        <v>60.047236</v>
+        <v>55.676149</v>
       </c>
       <c r="B305" t="n">
-        <v>30.451109</v>
+        <v>37.526259</v>
       </c>
     </row>
     <row r="306">
       <c r="A306" t="n">
-        <v>60.047236</v>
+        <v>55.755864</v>
       </c>
       <c r="B306" t="n">
-        <v>30.451109</v>
+        <v>37.617698</v>
       </c>
     </row>
     <row r="307">
       <c r="A307" t="n">
-        <v>59.890947</v>
+        <v>55.697772</v>
       </c>
       <c r="B307" t="n">
-        <v>30.266883</v>
+        <v>37.859219</v>
       </c>
     </row>
     <row r="308">
       <c r="A308" t="n">
-        <v>59.810242</v>
+        <v>55.702769</v>
       </c>
       <c r="B308" t="n">
-        <v>30.174392</v>
+        <v>37.651681</v>
       </c>
     </row>
     <row r="309">
       <c r="A309" t="n">
-        <v>59.929939</v>
+        <v>55.718699</v>
       </c>
       <c r="B309" t="n">
-        <v>30.350049</v>
+        <v>37.428037</v>
       </c>
     </row>
     <row r="310">
       <c r="A310" t="n">
-        <v>60.055493</v>
+        <v>55.711366</v>
       </c>
       <c r="B310" t="n">
-        <v>29.976053</v>
+        <v>37.767905</v>
       </c>
     </row>
     <row r="311">
       <c r="A311" t="n">
-        <v>59.92855</v>
+        <v>55.721752</v>
       </c>
       <c r="B311" t="n">
-        <v>30.24756</v>
+        <v>37.648843</v>
       </c>
     </row>
     <row r="312">
       <c r="A312" t="n">
-        <v>59.901247</v>
+        <v>55.614877</v>
       </c>
       <c r="B312" t="n">
-        <v>30.487698</v>
+        <v>37.750963</v>
       </c>
     </row>
     <row r="313">
       <c r="A313" t="n">
-        <v>59.882324</v>
+        <v>55.736194</v>
       </c>
       <c r="B313" t="n">
-        <v>29.890363</v>
+        <v>37.399506</v>
       </c>
     </row>
     <row r="314">
       <c r="A314" t="n">
-        <v>59.990579</v>
+        <v>55.719845</v>
       </c>
       <c r="B314" t="n">
-        <v>30.262059</v>
+        <v>37.660072</v>
       </c>
     </row>
     <row r="315">
       <c r="A315" t="n">
-        <v>59.874575</v>
+        <v>55.703586</v>
       </c>
       <c r="B315" t="n">
-        <v>30.443752</v>
+        <v>37.47333</v>
       </c>
     </row>
     <row r="316">
       <c r="A316" t="n">
-        <v>59.960179</v>
+        <v>55.710864</v>
       </c>
       <c r="B316" t="n">
-        <v>30.22883</v>
+        <v>37.770969</v>
       </c>
     </row>
     <row r="317">
       <c r="A317" t="n">
-        <v>59.941615</v>
+        <v>55.772284</v>
       </c>
       <c r="B317" t="n">
-        <v>30.351693</v>
+        <v>37.531819</v>
       </c>
     </row>
     <row r="318">
       <c r="A318" t="n">
-        <v>59.819115</v>
+        <v>55.841438</v>
       </c>
       <c r="B318" t="n">
-        <v>29.981156</v>
+        <v>37.459424</v>
       </c>
     </row>
     <row r="319">
       <c r="A319" t="n">
-        <v>59.843335</v>
+        <v>55.615151</v>
       </c>
       <c r="B319" t="n">
-        <v>30.021858</v>
+        <v>37.621417</v>
       </c>
     </row>
     <row r="320">
       <c r="A320" t="n">
-        <v>59.873451</v>
+        <v>55.71555</v>
       </c>
       <c r="B320" t="n">
-        <v>30.384014</v>
+        <v>37.771544</v>
       </c>
     </row>
     <row r="321">
       <c r="A321" t="n">
-        <v>59.940402</v>
+        <v>55.780841</v>
       </c>
       <c r="B321" t="n">
-        <v>30.264287</v>
+        <v>37.829799</v>
       </c>
     </row>
     <row r="322">
       <c r="A322" t="n">
-        <v>60.150415</v>
+        <v>55.713268</v>
       </c>
       <c r="B322" t="n">
-        <v>29.927877</v>
+        <v>37.612659</v>
       </c>
     </row>
     <row r="323">
       <c r="A323" t="n">
-        <v>59.727921</v>
+        <v>55.713547</v>
       </c>
       <c r="B323" t="n">
-        <v>30.09597</v>
+        <v>37.777715</v>
       </c>
     </row>
     <row r="324">
       <c r="A324" t="n">
-        <v>59.85139</v>
+        <v>55.539594</v>
       </c>
       <c r="B324" t="n">
-        <v>30.339458</v>
+        <v>37.54294</v>
       </c>
     </row>
     <row r="325">
       <c r="A325" t="n">
-        <v>59.877958</v>
+        <v>55.823186</v>
       </c>
       <c r="B325" t="n">
-        <v>30.482012</v>
+        <v>37.504492</v>
       </c>
     </row>
     <row r="326">
       <c r="A326" t="n">
-        <v>59.813346</v>
+        <v>55.645847</v>
       </c>
       <c r="B326" t="n">
-        <v>30.056066</v>
+        <v>37.560691</v>
       </c>
     </row>
     <row r="327">
       <c r="A327" t="n">
-        <v>59.940889</v>
+        <v>55.665756</v>
       </c>
       <c r="B327" t="n">
-        <v>30.289494</v>
+        <v>37.424929</v>
       </c>
     </row>
     <row r="328">
       <c r="A328" t="n">
-        <v>60.084733</v>
+        <v>55.572075</v>
       </c>
       <c r="B328" t="n">
-        <v>30.267395</v>
+        <v>37.571255</v>
       </c>
     </row>
     <row r="329">
       <c r="A329" t="n">
-        <v>60.015709</v>
+        <v>55.755864</v>
       </c>
       <c r="B329" t="n">
-        <v>30.294039</v>
+        <v>37.617698</v>
       </c>
     </row>
     <row r="330">
       <c r="A330" t="n">
-        <v>59.945603</v>
+        <v>55.764678</v>
       </c>
       <c r="B330" t="n">
-        <v>30.706204</v>
+        <v>37.636805</v>
       </c>
     </row>
     <row r="331">
       <c r="A331" t="n">
-        <v>59.917804</v>
+        <v>55.70809</v>
       </c>
       <c r="B331" t="n">
-        <v>30.278202</v>
+        <v>37.447961</v>
       </c>
     </row>
     <row r="332">
       <c r="A332" t="n">
-        <v>59.929687</v>
+        <v>55.762566</v>
       </c>
       <c r="B332" t="n">
-        <v>30.472355</v>
+        <v>37.66097</v>
       </c>
     </row>
     <row r="333">
       <c r="A333" t="n">
-        <v>59.987046</v>
+        <v>55.775459</v>
       </c>
       <c r="B333" t="n">
-        <v>30.314691</v>
+        <v>37.628406</v>
       </c>
     </row>
     <row r="334">
       <c r="A334" t="n">
-        <v>60.066096</v>
+        <v>55.659581</v>
       </c>
       <c r="B334" t="n">
-        <v>30.302402</v>
+        <v>37.759371</v>
       </c>
     </row>
     <row r="335">
       <c r="A335" t="n">
-        <v>59.953493</v>
+        <v>55.633023</v>
       </c>
       <c r="B335" t="n">
-        <v>30.221823</v>
+        <v>37.522764</v>
       </c>
     </row>
     <row r="336">
       <c r="A336" t="n">
-        <v>60.286924</v>
+        <v>55.724733</v>
       </c>
       <c r="B336" t="n">
-        <v>29.745977</v>
+        <v>37.664518</v>
       </c>
     </row>
     <row r="337">
       <c r="A337" t="n">
-        <v>59.954264</v>
+        <v>55.653015</v>
       </c>
       <c r="B337" t="n">
-        <v>30.41435</v>
+        <v>37.738099</v>
       </c>
     </row>
     <row r="338">
       <c r="A338" t="n">
-        <v>59.910875</v>
+        <v>55.681438</v>
       </c>
       <c r="B338" t="n">
-        <v>30.318015</v>
+        <v>37.900811</v>
       </c>
     </row>
     <row r="339">
       <c r="A339" t="n">
-        <v>59.9583</v>
+        <v>55.807273</v>
       </c>
       <c r="B339" t="n">
-        <v>30.30225</v>
+        <v>37.623843</v>
       </c>
     </row>
     <row r="340">
       <c r="A340" t="n">
-        <v>59.959899</v>
+        <v>55.817087</v>
       </c>
       <c r="B340" t="n">
-        <v>30.288443</v>
+        <v>37.649597</v>
       </c>
     </row>
     <row r="341">
       <c r="A341" t="n">
-        <v>60.085245</v>
+        <v>55.765422</v>
       </c>
       <c r="B341" t="n">
-        <v>30.267197</v>
+        <v>37.617195</v>
       </c>
     </row>
     <row r="342">
       <c r="A342" t="n">
-        <v>60.010375</v>
+        <v>55.842019</v>
       </c>
       <c r="B342" t="n">
-        <v>30.611351</v>
+        <v>37.551735</v>
       </c>
     </row>
     <row r="343">
       <c r="A343" t="n">
-        <v>60.041067</v>
+        <v>55.684072</v>
       </c>
       <c r="B343" t="n">
-        <v>30.645981</v>
+        <v>37.433535</v>
       </c>
     </row>
     <row r="344">
       <c r="A344" t="n">
-        <v>60.01096</v>
+        <v>55.721138</v>
       </c>
       <c r="B344" t="n">
-        <v>30.650221</v>
+        <v>37.402983</v>
       </c>
     </row>
     <row r="345">
       <c r="A345" t="n">
-        <v>60.141676</v>
+        <v>55.807481</v>
       </c>
       <c r="B345" t="n">
-        <v>30.210819</v>
+        <v>37.559658</v>
       </c>
     </row>
     <row r="346">
       <c r="A346" t="n">
-        <v>60.149927</v>
+        <v>55.777889</v>
       </c>
       <c r="B346" t="n">
-        <v>30.511979</v>
+        <v>37.588215</v>
       </c>
     </row>
     <row r="347">
       <c r="A347" t="n">
-        <v>60.042572</v>
+        <v>55.888614</v>
       </c>
       <c r="B347" t="n">
-        <v>30.301585</v>
+        <v>37.600774</v>
       </c>
     </row>
     <row r="348">
       <c r="A348" t="n">
-        <v>60.123053</v>
+        <v>55.896024</v>
       </c>
       <c r="B348" t="n">
-        <v>30.169793</v>
+        <v>37.619809</v>
       </c>
     </row>
     <row r="349">
       <c r="A349" t="n">
-        <v>59.950447</v>
+        <v>55.745068</v>
       </c>
       <c r="B349" t="n">
-        <v>30.249474</v>
+        <v>37.647612</v>
       </c>
     </row>
     <row r="350">
       <c r="A350" t="n">
-        <v>60.531715</v>
+        <v>55.845127</v>
       </c>
       <c r="B350" t="n">
-        <v>30.01699</v>
+        <v>37.53605</v>
       </c>
     </row>
     <row r="351">
       <c r="A351" t="n">
-        <v>59.922242</v>
+        <v>55.739422</v>
       </c>
       <c r="B351" t="n">
-        <v>30.347399</v>
+        <v>37.342894</v>
       </c>
     </row>
     <row r="352">
       <c r="A352" t="n">
-        <v>59.940276</v>
+        <v>55.691993</v>
       </c>
       <c r="B352" t="n">
-        <v>30.673568</v>
+        <v>37.465739</v>
       </c>
     </row>
     <row r="353">
       <c r="A353" t="n">
-        <v>59.987118</v>
+        <v>55.703682</v>
       </c>
       <c r="B353" t="n">
-        <v>30.234157</v>
+        <v>37.794181</v>
       </c>
     </row>
     <row r="354">
       <c r="A354" t="n">
-        <v>59.839936</v>
+        <v>55.877258</v>
       </c>
       <c r="B354" t="n">
-        <v>29.896633</v>
+        <v>37.32535</v>
       </c>
     </row>
     <row r="355">
       <c r="A355" t="n">
-        <v>59.88962</v>
+        <v>55.718699</v>
       </c>
       <c r="B355" t="n">
-        <v>30.379136</v>
+        <v>37.428037</v>
       </c>
     </row>
     <row r="356">
       <c r="A356" t="n">
-        <v>59.903733</v>
+        <v>55.718699</v>
       </c>
       <c r="B356" t="n">
-        <v>30.56498</v>
+        <v>37.428037</v>
       </c>
     </row>
     <row r="357">
       <c r="A357" t="n">
-        <v>60.047236</v>
+        <v>55.737213</v>
       </c>
       <c r="B357" t="n">
-        <v>30.451109</v>
+        <v>37.493084</v>
       </c>
     </row>
     <row r="358">
       <c r="A358" t="n">
-        <v>59.919973</v>
+        <v>55.861333</v>
       </c>
       <c r="B358" t="n">
-        <v>30.345629</v>
+        <v>37.322539</v>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" t="n">
+        <v>55.706847</v>
+      </c>
+      <c r="B359" t="n">
+        <v>37.606406</v>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" t="n">
+        <v>55.720869</v>
+      </c>
+      <c r="B360" t="n">
+        <v>37.574687</v>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" t="n">
+        <v>55.730269</v>
+      </c>
+      <c r="B361" t="n">
+        <v>37.771849</v>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" t="n">
+        <v>55.864162</v>
+      </c>
+      <c r="B362" t="n">
+        <v>37.474354</v>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" t="n">
+        <v>55.794092</v>
+      </c>
+      <c r="B363" t="n">
+        <v>37.789483</v>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" t="n">
+        <v>55.890997</v>
+      </c>
+      <c r="B364" t="n">
+        <v>37.617096</v>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" t="n">
+        <v>55.731237</v>
+      </c>
+      <c r="B365" t="n">
+        <v>37.474426</v>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" t="n">
+        <v>55.755819</v>
+      </c>
+      <c r="B366" t="n">
+        <v>37.617644</v>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" t="n">
+        <v>55.710524</v>
+      </c>
+      <c r="B367" t="n">
+        <v>37.41829</v>
+      </c>
+    </row>
+    <row r="368">
+      <c r="A368" t="n">
+        <v>55.655579</v>
+      </c>
+      <c r="B368" t="n">
+        <v>37.898071</v>
+      </c>
+    </row>
+    <row r="369">
+      <c r="A369" t="n">
+        <v>55.638186</v>
+      </c>
+      <c r="B369" t="n">
+        <v>37.794792</v>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" t="n">
+        <v>55.898664</v>
+      </c>
+      <c r="B370" t="n">
+        <v>37.276563</v>
+      </c>
+    </row>
+    <row r="371">
+      <c r="A371" t="n">
+        <v>55.70002</v>
+      </c>
+      <c r="B371" t="n">
+        <v>37.505157</v>
+      </c>
+    </row>
+    <row r="372">
+      <c r="A372" t="n">
+        <v>55.755864</v>
+      </c>
+      <c r="B372" t="n">
+        <v>37.617698</v>
+      </c>
+    </row>
+    <row r="373">
+      <c r="A373" t="n">
+        <v>55.557037</v>
+      </c>
+      <c r="B373" t="n">
+        <v>37.70876</v>
+      </c>
+    </row>
+    <row r="374">
+      <c r="A374" t="n">
+        <v>55.720413</v>
+      </c>
+      <c r="B374" t="n">
+        <v>37.862633</v>
+      </c>
+    </row>
+    <row r="375">
+      <c r="A375" t="n">
+        <v>55.793541</v>
+      </c>
+      <c r="B375" t="n">
+        <v>37.803281</v>
+      </c>
+    </row>
+    <row r="376">
+      <c r="A376" t="n">
+        <v>55.638247</v>
+      </c>
+      <c r="B376" t="n">
+        <v>37.75656</v>
+      </c>
+    </row>
+    <row r="377">
+      <c r="A377" t="n">
+        <v>55.896337</v>
+      </c>
+      <c r="B377" t="n">
+        <v>37.609146</v>
+      </c>
+    </row>
+    <row r="378">
+      <c r="A378" t="n">
+        <v>55.877642</v>
+      </c>
+      <c r="B378" t="n">
+        <v>37.52068</v>
+      </c>
+    </row>
+    <row r="379">
+      <c r="A379" t="n">
+        <v>55.897902</v>
+      </c>
+      <c r="B379" t="n">
+        <v>37.6047</v>
+      </c>
+    </row>
+    <row r="380">
+      <c r="A380" t="n">
+        <v>55.889593</v>
+      </c>
+      <c r="B380" t="n">
+        <v>37.527328</v>
+      </c>
+    </row>
+    <row r="381">
+      <c r="A381" t="n">
+        <v>55.89823</v>
+      </c>
+      <c r="B381" t="n">
+        <v>37.571965</v>
+      </c>
+    </row>
+    <row r="382">
+      <c r="A382" t="n">
+        <v>55.782694</v>
+      </c>
+      <c r="B382" t="n">
+        <v>37.354995</v>
+      </c>
+    </row>
+    <row r="383">
+      <c r="A383" t="n">
+        <v>55.765154</v>
+      </c>
+      <c r="B383" t="n">
+        <v>37.776646</v>
+      </c>
+    </row>
+    <row r="384">
+      <c r="A384" t="n">
+        <v>55.863863</v>
+      </c>
+      <c r="B384" t="n">
+        <v>37.701709</v>
+      </c>
+    </row>
+    <row r="385">
+      <c r="A385" t="n">
+        <v>55.742747</v>
+      </c>
+      <c r="B385" t="n">
+        <v>37.632143</v>
+      </c>
+    </row>
+    <row r="386">
+      <c r="A386" t="n">
+        <v>55.836838</v>
+      </c>
+      <c r="B386" t="n">
+        <v>38.411755</v>
+      </c>
+    </row>
+    <row r="387">
+      <c r="A387" t="n">
+        <v>55.931255</v>
+      </c>
+      <c r="B387" t="n">
+        <v>37.496246</v>
+      </c>
+    </row>
+    <row r="388">
+      <c r="A388" t="n">
+        <v>55.895782</v>
+      </c>
+      <c r="B388" t="n">
+        <v>37.711842</v>
+      </c>
+    </row>
+    <row r="389">
+      <c r="A389" t="n">
+        <v>55.919559</v>
+      </c>
+      <c r="B389" t="n">
+        <v>38.008995</v>
+      </c>
+    </row>
+    <row r="390">
+      <c r="A390" t="n">
+        <v>55.642738</v>
+      </c>
+      <c r="B390" t="n">
+        <v>37.793624</v>
+      </c>
+    </row>
+    <row r="391">
+      <c r="A391" t="n">
+        <v>55.942766</v>
+      </c>
+      <c r="B391" t="n">
+        <v>37.552058</v>
+      </c>
+    </row>
+    <row r="392">
+      <c r="A392" t="n">
+        <v>55.859443</v>
+      </c>
+      <c r="B392" t="n">
+        <v>37.568479</v>
+      </c>
+    </row>
+    <row r="393">
+      <c r="A393" t="n">
+        <v>55.680747</v>
+      </c>
+      <c r="B393" t="n">
+        <v>37.763405</v>
+      </c>
+    </row>
+    <row r="394">
+      <c r="A394" t="n">
+        <v>55.670854</v>
+      </c>
+      <c r="B394" t="n">
+        <v>37.747496</v>
+      </c>
+    </row>
+    <row r="395">
+      <c r="A395" t="n">
+        <v>55.732175</v>
+      </c>
+      <c r="B395" t="n">
+        <v>37.417536</v>
+      </c>
+    </row>
+    <row r="396">
+      <c r="A396" t="n">
+        <v>55.555958</v>
+      </c>
+      <c r="B396" t="n">
+        <v>37.709901</v>
+      </c>
+    </row>
+    <row r="397">
+      <c r="A397" t="n">
+        <v>55.913263</v>
+      </c>
+      <c r="B397" t="n">
+        <v>37.842978</v>
+      </c>
+    </row>
+    <row r="398">
+      <c r="A398" t="n">
+        <v>55.610478</v>
+      </c>
+      <c r="B398" t="n">
+        <v>37.292436</v>
+      </c>
+    </row>
+    <row r="399">
+      <c r="A399" t="n">
+        <v>56.043005</v>
+      </c>
+      <c r="B399" t="n">
+        <v>37.852868</v>
+      </c>
+    </row>
+    <row r="400">
+      <c r="A400" t="n">
+        <v>55.589671</v>
+      </c>
+      <c r="B400" t="n">
+        <v>38.136224</v>
+      </c>
+    </row>
+    <row r="401">
+      <c r="A401" t="n">
+        <v>55.632916</v>
+      </c>
+      <c r="B401" t="n">
+        <v>38.069694</v>
+      </c>
+    </row>
+    <row r="402">
+      <c r="A402" t="n">
+        <v>55.589743</v>
+      </c>
+      <c r="B402" t="n">
+        <v>37.900542</v>
+      </c>
+    </row>
+    <row r="403">
+      <c r="A403" t="n">
+        <v>55.566028</v>
+      </c>
+      <c r="B403" t="n">
+        <v>37.935351</v>
+      </c>
+    </row>
+    <row r="404">
+      <c r="A404" t="n">
+        <v>55.325206</v>
+      </c>
+      <c r="B404" t="n">
+        <v>37.851116</v>
+      </c>
+    </row>
+    <row r="405">
+      <c r="A405" t="n">
+        <v>55.3235</v>
+      </c>
+      <c r="B405" t="n">
+        <v>37.892951</v>
+      </c>
+    </row>
+    <row r="406">
+      <c r="A406" t="n">
+        <v>55.671097</v>
+      </c>
+      <c r="B406" t="n">
+        <v>37.269305</v>
+      </c>
+    </row>
+    <row r="407">
+      <c r="A407" t="n">
+        <v>55.841043</v>
+      </c>
+      <c r="B407" t="n">
+        <v>37.256225</v>
+      </c>
+    </row>
+    <row r="408">
+      <c r="A408" t="n">
+        <v>55.892617</v>
+      </c>
+      <c r="B408" t="n">
+        <v>37.453765</v>
+      </c>
+    </row>
+    <row r="409">
+      <c r="A409" t="n">
+        <v>55.942499</v>
+      </c>
+      <c r="B409" t="n">
+        <v>37.281117</v>
+      </c>
+    </row>
+    <row r="410">
+      <c r="A410" t="n">
+        <v>56.046308</v>
+      </c>
+      <c r="B410" t="n">
+        <v>37.479582</v>
+      </c>
+    </row>
+    <row r="411">
+      <c r="A411" t="n">
+        <v>55.812545</v>
+      </c>
+      <c r="B411" t="n">
+        <v>37.958564</v>
+      </c>
+    </row>
+    <row r="412">
+      <c r="A412" t="n">
+        <v>55.499183</v>
+      </c>
+      <c r="B412" t="n">
+        <v>37.485601</v>
+      </c>
+    </row>
+    <row r="413">
+      <c r="A413" t="n">
+        <v>55.857397</v>
+      </c>
+      <c r="B413" t="n">
+        <v>37.113968</v>
+      </c>
+    </row>
+    <row r="414">
+      <c r="A414" t="n">
+        <v>55.738718</v>
+      </c>
+      <c r="B414" t="n">
+        <v>36.982679</v>
+      </c>
+    </row>
+    <row r="415">
+      <c r="A415" t="n">
+        <v>55.848817</v>
+      </c>
+      <c r="B415" t="n">
+        <v>37.170247</v>
+      </c>
+    </row>
+    <row r="416">
+      <c r="A416" t="n">
+        <v>55.812403</v>
+      </c>
+      <c r="B416" t="n">
+        <v>37.083874</v>
+      </c>
+    </row>
+    <row r="417">
+      <c r="A417" t="n">
+        <v>55.41284</v>
+      </c>
+      <c r="B417" t="n">
+        <v>37.533751</v>
+      </c>
+    </row>
+    <row r="418">
+      <c r="A418" t="n">
+        <v>55.409692</v>
+      </c>
+      <c r="B418" t="n">
+        <v>37.545087</v>
+      </c>
+    </row>
+    <row r="419">
+      <c r="A419" t="n">
+        <v>55.440345</v>
+      </c>
+      <c r="B419" t="n">
+        <v>37.489796</v>
+      </c>
+    </row>
+    <row r="420">
+      <c r="A420" t="n">
+        <v>55.457592</v>
+      </c>
+      <c r="B420" t="n">
+        <v>37.580202</v>
+      </c>
+    </row>
+    <row r="421">
+      <c r="A421" t="n">
+        <v>55.347357</v>
+      </c>
+      <c r="B421" t="n">
+        <v>37.554582</v>
+      </c>
+    </row>
+    <row r="422">
+      <c r="A422" t="n">
+        <v>55.310227</v>
+      </c>
+      <c r="B422" t="n">
+        <v>37.521686</v>
+      </c>
+    </row>
+    <row r="423">
+      <c r="A423" t="n">
+        <v>55.672534</v>
+      </c>
+      <c r="B423" t="n">
+        <v>37.037979</v>
+      </c>
+    </row>
+    <row r="424">
+      <c r="A424" t="n">
+        <v>55.624556</v>
+      </c>
+      <c r="B424" t="n">
+        <v>37.866891</v>
+      </c>
+    </row>
+    <row r="425">
+      <c r="A425" t="n">
+        <v>55.755819</v>
+      </c>
+      <c r="B425" t="n">
+        <v>37.617644</v>
+      </c>
+    </row>
+    <row r="426">
+      <c r="A426" t="n">
+        <v>55.731445</v>
+      </c>
+      <c r="B426" t="n">
+        <v>37.474363</v>
       </c>
     </row>
   </sheetData>

</xml_diff>